<commit_message>
Add images, fix liking bug
</commit_message>
<xml_diff>
--- a/backend/data/Competitors.xlsx
+++ b/backend/data/Competitors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Competitors-Male" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="265">
   <si>
     <t xml:space="preserve">Player</t>
   </si>
@@ -96,6 +96,12 @@
     <t xml:space="preserve">Libema Winning Year</t>
   </si>
   <si>
+    <t xml:space="preserve">ImageURL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
     <t xml:space="preserve">Daniil Medvedev</t>
   </si>
   <si>
@@ -120,6 +126,12 @@
     <t xml:space="preserve">Gilles Cervara</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/medvedev-full-2022-may.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
     <t xml:space="preserve">Felix Auger-Aliassime</t>
   </si>
   <si>
@@ -141,6 +153,9 @@
     <t xml:space="preserve">Frederic Fontang, Toni Nadal</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/auger-aliassime-full-2022-may-new.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Borna Coric</t>
   </si>
   <si>
@@ -156,6 +171,9 @@
     <t xml:space="preserve">Mate Delic</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/coric-full-2022-may.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alex de Minaur</t>
   </si>
   <si>
@@ -171,6 +189,9 @@
     <t xml:space="preserve">Adolfo Gutierrez</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/deminaur-full-2022-june-final.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pablo Carreno Busta</t>
   </si>
   <si>
@@ -186,6 +207,9 @@
     <t xml:space="preserve">Samuel Lopez, Jose Antonio Sanchez-de Luna</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/carreno-busta-full-2022-may.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marin Cilic</t>
   </si>
   <si>
@@ -201,6 +225,27 @@
     <t xml:space="preserve">Ivan Cinkus, Vilim Visak</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://libema-open.nl/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/wp-content/uploads/2023/05/cilic-full-2022-may.png</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Roberto Bautista Agut</t>
   </si>
   <si>
@@ -213,6 +258,27 @@
     <t xml:space="preserve">Daniel Gimeno-Traver, Felix Mantilla</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://libema-open.nl/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">wp-content/uploads/2023/05/bautista-agut-full-2022-may.png</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Botic van de Zandschulp</t>
   </si>
   <si>
@@ -231,6 +297,27 @@
     <t xml:space="preserve">Peter Lucassen</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://libema-open.nl/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">wp-content/uploads/2023/05/van-de-zandschulp-full-2022-may.png</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Milos Raonic</t>
   </si>
   <si>
@@ -249,6 +336,9 @@
     <t xml:space="preserve">Comeback</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/raonic_full_ao20.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tallon Griekspoor</t>
   </si>
   <si>
@@ -261,6 +351,9 @@
     <t xml:space="preserve">Kristof Vliegen</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/griekspoor-full-2022-may.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Miomir Kecmanovic</t>
   </si>
   <si>
@@ -276,6 +369,9 @@
     <t xml:space="preserve">Wayne Black, Ivan Cinkus</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/kecmanovic_full_2022_october-1.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bernabe Zapata Miralles</t>
   </si>
   <si>
@@ -288,6 +384,9 @@
     <t xml:space="preserve">Samuel Ribeiro</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/zapata_miralles_full_2022.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maxime Cressy</t>
   </si>
   <si>
@@ -303,6 +402,9 @@
     <t xml:space="preserve">Alexandre Sidorenko, Juanjo Climent, Andrew Mawire </t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/cressy-full-2022-june.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emil Ruusuvuori</t>
   </si>
   <si>
@@ -318,6 +420,9 @@
     <t xml:space="preserve">Federico Ricci</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/ruusuvuori_full_2023.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adrian Mannarino</t>
   </si>
   <si>
@@ -339,6 +444,9 @@
     <t xml:space="preserve">Erwann Tortuyaux</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/mannarino-full-2022-may.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brandon Nakashima</t>
   </si>
   <si>
@@ -351,6 +459,9 @@
     <t xml:space="preserve">Edwardo Infantino</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/nakashima-full-2022-may.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alexander Bublik</t>
   </si>
   <si>
@@ -366,6 +477,9 @@
     <t xml:space="preserve">Artem Suprunov</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/bublik_full_2023_update.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ugo Humbert</t>
   </si>
   <si>
@@ -378,6 +492,9 @@
     <t xml:space="preserve">Jeremy Chardy</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/humbert-full-2022-june.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mikael Ymer</t>
   </si>
   <si>
@@ -393,6 +510,9 @@
     <t xml:space="preserve">Daniel Berta</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/ymer_m_full_ao20.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tim van Rijthoven</t>
   </si>
   <si>
@@ -408,6 +528,9 @@
     <t xml:space="preserve">Igor Sijsling</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2022/05/van_rijthoven_tim_head_pp19.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Belinda Bencic</t>
   </si>
   <si>
@@ -420,6 +543,12 @@
     <t xml:space="preserve">Bencic possesses a versatile game marked by excellent court coverage and an ability to change direction of the ball with ease. Her smart tactical sense allows her to construct points effectively, often outmaneuvering her opponents with precise shot placement.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Bencic_Hero-Smile.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
     <t xml:space="preserve">Veronika Kudermetova</t>
   </si>
   <si>
@@ -432,6 +561,9 @@
     <t xml:space="preserve">Sergey Demekhine, Vladimir Platenik</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Kudermetova_Hero-Smile.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Liudmila Samsonova</t>
   </si>
   <si>
@@ -441,6 +573,9 @@
     <t xml:space="preserve">Samsonova is known for her aggressive game. She has powerful groundstrokes from both wings and a strong serve, which allows her to dictate play and keep opponents on the back foot.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Samsonova_Crop.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Victoria Azarenka</t>
   </si>
   <si>
@@ -453,6 +588,9 @@
     <t xml:space="preserve">Maxime Tchoutakian</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/azarenka.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Qinwen Zheng</t>
   </si>
   <si>
@@ -468,6 +606,9 @@
     <t xml:space="preserve">Pedro Riba Madrid</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Zheng-Torso_328120.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ekaterina Alexandrova</t>
   </si>
   <si>
@@ -480,6 +621,9 @@
     <t xml:space="preserve">Evgeny Alexandrova</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Alexandrova_Hero-Smile.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Elise Mertens</t>
   </si>
   <si>
@@ -495,6 +639,9 @@
     <t xml:space="preserve">Alexander Kneepkens</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Mertens_Hero-Smile.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Petra Martic</t>
   </si>
   <si>
@@ -507,6 +654,9 @@
     <t xml:space="preserve">Michael Geserer</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Martic_Hero-Smile.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bianca Andreescu</t>
   </si>
   <si>
@@ -519,6 +669,9 @@
     <t xml:space="preserve">Christphe Lambert</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Andreescu_crop.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shelby Rogers</t>
   </si>
   <si>
@@ -531,16 +684,7 @@
     <t xml:space="preserve">Piotr Sierzputowski</t>
   </si>
   <si>
-    <t xml:space="preserve">Paula Badosa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fighter, personality (magazines, TV shows, etc.), groundstrokes, consistency, serve, aggressive, footwork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Badosa is a consistent baseline player with a strong forehand. She has a patient game style, often waiting for the right opportunity to attack.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jorge Garcia</t>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Rogers-Torso_317421.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Marie Bouzkova</t>
@@ -558,6 +702,9 @@
     <t xml:space="preserve">Cristian Requeni, Milan Bouzek</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/QcvLKQRa.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aliaksandra Sasnovich</t>
   </si>
   <si>
@@ -573,6 +720,9 @@
     <t xml:space="preserve">Dzmitry Klimenko</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/MLBGcqtM.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Varvara Gracheva</t>
   </si>
   <si>
@@ -585,6 +735,9 @@
     <t xml:space="preserve">Xavier Pujo</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Gracheva_crop.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Karolina Muchova</t>
   </si>
   <si>
@@ -597,6 +750,9 @@
     <t xml:space="preserve">David Kotyza</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Muchova_Hero-Smile.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Caty Mcnally</t>
   </si>
   <si>
@@ -609,6 +765,9 @@
     <t xml:space="preserve">Kevin O’Neill</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/McNally_Crop.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anna Blinkova</t>
   </si>
   <si>
@@ -618,6 +777,9 @@
     <t xml:space="preserve">Anna Blinkova is a solid all-court player known for her powerful groundstrokes. Her aggressive style of play often sees her taking the ball on the rise and aiming for the lines. Blinkova has shown that she can compete at the top level and has recorded victories against higher-ranked opponents. Her ability to generate power from both wings and her willingness to attack and dictate play are key elements of her game.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/LiQQMObq.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Evgeniya Rodina</t>
   </si>
   <si>
@@ -630,6 +792,9 @@
     <t xml:space="preserve">Oxana Mishikova</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/KxenXejL.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alison Riske-Amritraj</t>
   </si>
   <si>
@@ -642,6 +807,9 @@
     <t xml:space="preserve">Thomas Gutteridge</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/SuWqgWYb.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ysaline Bonaventure</t>
   </si>
   <si>
@@ -654,6 +822,9 @@
     <t xml:space="preserve">Hugo Guerriero</t>
   </si>
   <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/fNpQoEOl.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rebecca Peterson</t>
   </si>
   <si>
@@ -664,6 +835,27 @@
   </si>
   <si>
     <t xml:space="preserve">Mart Peterson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/ODTCCbpp.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anna-Lena Friedsam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">groundstrokes, aggressive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anna-Lena Friedsam is an aggressive baseliner who relies on her powerful groundstrokes to dictate play. She looks to take control of the rallies by hitting aggressive shots and going for winners. At the same time, she has the ability to defend and counter-punch effectively, adjusting her game according to the situation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrice Hopfe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Friedsam_Crop.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Elina Svitolina</t>
@@ -693,7 +885,7 @@
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -714,6 +906,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -764,7 +963,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -781,11 +980,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -881,14 +1084,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W1021"/>
+  <dimension ref="A1:Y1021"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R2" activeCellId="0" sqref="R2"/>
+      <selection pane="bottomRight" activeCell="Y2" activeCellId="0" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -901,6 +1104,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="18.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,16 +1177,22 @@
       <c r="W1" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="X1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>27</v>
@@ -991,19 +1201,19 @@
         <v>198</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L2" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1035,7 +1245,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="U2" s="0" t="str">
         <f aca="false">IF(B2=M2,"All time high","")</f>
@@ -1045,16 +1255,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>22</v>
@@ -1063,22 +1279,22 @@
         <v>193</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L3" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1110,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="U3" s="0" t="str">
         <f aca="false">IF(B3=M3,"All time high","")</f>
@@ -1120,16 +1336,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>26</v>
@@ -1138,22 +1360,22 @@
         <v>188</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="L4" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1185,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="U4" s="0" t="str">
         <f aca="false">IF(B4=M4,"All time high","")</f>
@@ -1195,16 +1417,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>24</v>
@@ -1213,22 +1441,22 @@
         <v>183</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="L5" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -1260,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="U5" s="0" t="str">
         <f aca="false">IF(B5=M5,"All time high","")</f>
@@ -1270,16 +1498,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>31</v>
@@ -1288,22 +1522,22 @@
         <v>188</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="L6" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1335,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="U6" s="0" t="str">
         <f aca="false">IF(B6=M6,"All time high","")</f>
@@ -1345,16 +1579,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>34</v>
@@ -1363,22 +1603,22 @@
         <v>198</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="L7" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -1410,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="U7" s="0" t="str">
         <f aca="false">IF(B7=M7,"All time high","")</f>
@@ -1420,16 +1660,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y7" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>35</v>
@@ -1438,22 +1684,22 @@
         <v>193</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="M8" s="0" t="n">
         <v>9</v>
@@ -1481,7 +1727,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="U8" s="0" t="str">
         <f aca="false">IF(B8=M8,"All time high","")</f>
@@ -1493,16 +1739,22 @@
       <c r="W8" s="0" t="n">
         <v>2014</v>
       </c>
+      <c r="X8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y8" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>27</v>
@@ -1511,22 +1763,22 @@
         <v>191</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="L9" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1558,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="T9" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="U9" s="0" t="str">
         <f aca="false">IF(B9=M9,"All time high","")</f>
@@ -1568,16 +1820,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y9" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>32</v>
@@ -1586,22 +1844,22 @@
         <v>196</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="M10" s="0" t="n">
         <v>3</v>
@@ -1629,25 +1887,31 @@
         <v>0</v>
       </c>
       <c r="T10" s="0" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="V10" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y10" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>26</v>
@@ -1656,22 +1920,22 @@
         <v>188</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="L11" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1703,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="0" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="U11" s="0" t="str">
         <f aca="false">IF(B11=M11,"All time high","")</f>
@@ -1713,16 +1977,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y11" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>23</v>
@@ -1731,22 +2001,22 @@
         <v>183</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="L12" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1778,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="U12" s="0" t="str">
         <f aca="false">IF(B12=M12,"All time high","")</f>
@@ -1788,16 +2058,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y12" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>26</v>
@@ -1806,22 +2082,22 @@
         <v>183</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="L13" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1853,7 +2129,7 @@
         <v>1</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="U13" s="0" t="str">
         <f aca="false">IF(B13=M13,"All time high","")</f>
@@ -1863,16 +2139,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y13" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>26</v>
@@ -1881,22 +2163,22 @@
         <v>201</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="L14" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -1927,8 +2209,8 @@
         <f aca="false">IF(B14=M14,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T14" s="4" t="s">
-        <v>91</v>
+      <c r="T14" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="U14" s="0" t="str">
         <f aca="false">IF(B14=M14,"All time high","")</f>
@@ -1938,16 +2220,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y14" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>24</v>
@@ -1956,22 +2244,22 @@
         <v>188</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>95</v>
+        <v>110</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="L15" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2003,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="T15" s="0" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="U15" s="0" t="str">
         <f aca="false">IF(B15=M15,"All time high","")</f>
@@ -2013,16 +2301,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X15" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y15" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>37</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>34</v>
@@ -2031,22 +2325,22 @@
         <v>180</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="L16" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -2078,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="T16" s="0" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="U16" s="0" t="str">
         <f aca="false">IF(B16=M16,"All time high","")</f>
@@ -2091,16 +2385,22 @@
       <c r="W16" s="0" t="n">
         <v>2019</v>
       </c>
+      <c r="X16" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y16" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>52</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>21</v>
@@ -2109,22 +2409,22 @@
         <v>188</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="G17" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="L17" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2156,7 +2456,7 @@
         <v>0</v>
       </c>
       <c r="T17" s="0" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="U17" s="0" t="str">
         <f aca="false">IF(B17=M17,"All time high","")</f>
@@ -2166,16 +2466,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X17" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y17" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>48</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>25</v>
@@ -2184,22 +2490,22 @@
         <v>196</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="L18" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2231,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="0" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="U18" s="0" t="str">
         <f aca="false">IF(B18=M18,"All time high","")</f>
@@ -2241,16 +2547,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X18" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y18" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>24</v>
@@ -2259,22 +2571,22 @@
         <v>188</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="L19" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2306,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="T19" s="0" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="U19" s="0" t="str">
         <f aca="false">IF(B19=M19,"All time high","")</f>
@@ -2316,16 +2628,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X19" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y19" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>53</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>24</v>
@@ -2334,22 +2652,22 @@
         <v>183</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="L20" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2381,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="T20" s="0" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="U20" s="0" t="str">
         <f aca="false">IF(B20=M20,"All time high","")</f>
@@ -2391,16 +2709,22 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="X20" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y20" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>157</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>26</v>
@@ -2409,22 +2733,22 @@
         <v>188</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="L21" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -2456,7 +2780,7 @@
         <v>0</v>
       </c>
       <c r="T21" s="0" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="U21" s="0" t="str">
         <f aca="false">IF(B21=M21,"All time high","")</f>
@@ -2468,6 +2792,12 @@
       </c>
       <c r="W21" s="0" t="n">
         <v>2022</v>
+      </c>
+      <c r="X21" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y21" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5505,6 +5835,24 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="X6" r:id="rId1" display="https://libema-open.nl/wp-content/uploads/2023/05/carreno-busta-full-2022-may.png"/>
+    <hyperlink ref="X7" r:id="rId2" display="https://libema-open.nl/"/>
+    <hyperlink ref="X8" r:id="rId3" display="https://libema-open.nl/"/>
+    <hyperlink ref="X9" r:id="rId4" display="https://libema-open.nl/"/>
+    <hyperlink ref="X10" r:id="rId5" display="https://libema-open.nl/wp-content/uploads/2023/05/raonic_full_ao20.png"/>
+    <hyperlink ref="X11" r:id="rId6" display="https://libema-open.nl/wp-content/uploads/2023/05/griekspoor-full-2022-may.png"/>
+    <hyperlink ref="X12" r:id="rId7" display="https://libema-open.nl/wp-content/uploads/2023/05/kecmanovic_full_2022_october-1.png"/>
+    <hyperlink ref="X13" r:id="rId8" display="https://libema-open.nl/wp-content/uploads/2023/05/zapata_miralles_full_2022.png"/>
+    <hyperlink ref="X14" r:id="rId9" display="https://libema-open.nl/wp-content/uploads/2023/05/cressy-full-2022-june.png"/>
+    <hyperlink ref="X15" r:id="rId10" display="https://libema-open.nl/wp-content/uploads/2023/05/ruusuvuori_full_2023.png"/>
+    <hyperlink ref="X16" r:id="rId11" display="https://libema-open.nl/wp-content/uploads/2023/05/mannarino-full-2022-may.png"/>
+    <hyperlink ref="X17" r:id="rId12" display="https://libema-open.nl/wp-content/uploads/2023/05/nakashima-full-2022-may.png"/>
+    <hyperlink ref="X18" r:id="rId13" display="https://libema-open.nl/wp-content/uploads/2023/05/bublik_full_2023_update.png"/>
+    <hyperlink ref="X19" r:id="rId14" display="https://libema-open.nl/wp-content/uploads/2023/05/humbert-full-2022-june.png"/>
+    <hyperlink ref="X20" r:id="rId15" display="https://libema-open.nl/wp-content/uploads/2023/05/ymer_m_full_ao20.png"/>
+    <hyperlink ref="X21" r:id="rId16" display="https://libema-open.nl/wp-content/uploads/2022/05/van_rijthoven_tim_head_pp19.png"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5520,19 +5868,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="V3" activeCellId="0" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.34"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5599,16 +5948,22 @@
       <c r="U1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="V1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>26</v>
@@ -5617,19 +5972,19 @@
         <v>175</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="K2" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -5663,16 +6018,22 @@
       <c r="T2" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V2" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>131</v>
+      <c r="A3" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>26</v>
@@ -5681,16 +6042,16 @@
         <v>175</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>2</v>
@@ -5706,7 +6067,7 @@
         <v>11</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="Q3" s="3" t="b">
         <f aca="false">IF(B3&lt;11,TRUE(),FALSE())</f>
@@ -5723,16 +6084,22 @@
       <c r="T3" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>135</v>
+      <c r="A4" s="5" t="s">
+        <v>161</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>24</v>
@@ -5741,16 +6108,16 @@
         <v>182</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>12</v>
@@ -5780,16 +6147,22 @@
       <c r="T4" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V4" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>138</v>
+      <c r="A5" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>33</v>
@@ -5801,13 +6174,13 @@
         <v>8</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="K5" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -5826,8 +6199,8 @@
         <f aca="false">2023-N5</f>
         <v>20</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>141</v>
+      <c r="P5" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="Q5" s="3" t="b">
         <f aca="false">IF(B5&lt;11,TRUE(),FALSE())</f>
@@ -5844,16 +6217,22 @@
       <c r="T5" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V5" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>142</v>
+      <c r="A6" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>20</v>
@@ -5862,16 +6241,16 @@
         <v>178</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>19</v>
@@ -5886,8 +6265,8 @@
         <f aca="false">2023-N6</f>
         <v>5</v>
       </c>
-      <c r="P6" s="4" t="s">
-        <v>146</v>
+      <c r="P6" s="5" t="s">
+        <v>174</v>
       </c>
       <c r="Q6" s="3" t="b">
         <f aca="false">IF(B6&lt;11,TRUE(),FALSE())</f>
@@ -5904,16 +6283,22 @@
       <c r="T6" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V6" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>147</v>
+      <c r="A7" s="5" t="s">
+        <v>176</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>28</v>
@@ -5922,16 +6307,16 @@
         <v>175</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="K7" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -5951,7 +6336,7 @@
         <v>12</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="Q7" s="3" t="b">
         <f aca="false">IF(B7&lt;11,TRUE(),FALSE())</f>
@@ -5972,16 +6357,22 @@
       <c r="U7" s="0" t="n">
         <v>2022</v>
       </c>
+      <c r="V7" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>151</v>
+      <c r="A8" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>27</v>
@@ -5990,19 +6381,19 @@
         <v>179</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>1</v>
@@ -6017,8 +6408,8 @@
         <f aca="false">2023-N8</f>
         <v>13</v>
       </c>
-      <c r="P8" s="4" t="s">
-        <v>155</v>
+      <c r="P8" s="5" t="s">
+        <v>185</v>
       </c>
       <c r="Q8" s="3" t="b">
         <f aca="false">IF(B8&lt;11,TRUE(),FALSE())</f>
@@ -6035,16 +6426,22 @@
       <c r="T8" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V8" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="W8" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>156</v>
+      <c r="A9" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>32</v>
@@ -6053,19 +6450,19 @@
         <v>181</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>157</v>
+        <v>188</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>158</v>
+        <v>189</v>
       </c>
       <c r="K9" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -6085,7 +6482,7 @@
         <v>18</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="Q9" s="3" t="b">
         <f aca="false">IF(B9&lt;11,TRUE(),FALSE())</f>
@@ -6102,16 +6499,22 @@
       <c r="T9" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V9" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="W9" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>160</v>
+      <c r="A10" s="5" t="s">
+        <v>192</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>22</v>
@@ -6120,19 +6523,19 @@
         <v>170</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>162</v>
+        <v>194</v>
       </c>
       <c r="L10" s="0" t="n">
         <v>4</v>
@@ -6148,7 +6551,7 @@
         <v>8</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>163</v>
+        <v>195</v>
       </c>
       <c r="Q10" s="3" t="b">
         <f aca="false">IF(B10&lt;11,TRUE(),FALSE())</f>
@@ -6165,16 +6568,22 @@
       <c r="T10" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V10" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="W10" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>164</v>
+      <c r="A11" s="5" t="s">
+        <v>197</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>30</v>
@@ -6183,19 +6592,19 @@
         <v>175</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>166</v>
+        <v>199</v>
       </c>
       <c r="K11" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -6215,7 +6624,7 @@
         <v>14</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="Q11" s="3" t="b">
         <f aca="false">IF(B11&lt;11,TRUE(),FALSE())</f>
@@ -6232,53 +6641,59 @@
       <c r="T11" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V11" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="W11" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>168</v>
+      <c r="A12" s="5" t="s">
+        <v>202</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>180</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>169</v>
+        <v>204</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="M12" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="N12" s="0" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="O12" s="0" t="n">
         <f aca="false">2023-N12</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
       <c r="Q12" s="3" t="b">
         <f aca="false">IF(B12&lt;11,TRUE(),FALSE())</f>
@@ -6286,7 +6701,7 @@
       </c>
       <c r="R12" s="3" t="b">
         <f aca="false">IF(L12&lt;11,TRUE(),FALSE())</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12" s="3" t="b">
         <f aca="false">IF(B12=L12,TRUE(),FALSE())</f>
@@ -6295,53 +6710,60 @@
       <c r="T12" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>172</v>
+      <c r="V12" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="W12" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>180</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>8</v>
+        <v>209</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>174</v>
+        <v>210</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>175</v>
+        <v>211</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="M13" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>2013</v>
+        <v>2009</v>
       </c>
       <c r="O13" s="0" t="n">
         <f aca="false">2023-N13</f>
-        <v>10</v>
-      </c>
-      <c r="P13" s="0" t="s">
-        <v>176</v>
+        <v>14</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>212</v>
       </c>
       <c r="Q13" s="3" t="b">
         <f aca="false">IF(B13&lt;11,TRUE(),FALSE())</f>
@@ -6358,54 +6780,53 @@
       <c r="T13" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V13" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="W13" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>177</v>
+      <c r="A14" s="5" t="s">
+        <v>214</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>174</v>
-      </c>
-      <c r="G14" s="0" t="s">
         <v>178</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>179</v>
+        <v>215</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="K14" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>216</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="N14" s="0" t="n">
-        <v>2009</v>
+        <v>2016</v>
       </c>
       <c r="O14" s="0" t="n">
         <f aca="false">2023-N14</f>
-        <v>14</v>
-      </c>
-      <c r="P14" s="4" t="s">
-        <v>181</v>
+        <v>7</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>217</v>
       </c>
       <c r="Q14" s="3" t="b">
         <f aca="false">IF(B14&lt;11,TRUE(),FALSE())</f>
@@ -6422,47 +6843,59 @@
       <c r="T14" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V14" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="W14" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>182</v>
+      <c r="A15" s="5" t="s">
+        <v>219</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>178</v>
+        <v>180</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>116</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>183</v>
+        <v>220</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>184</v>
+        <v>221</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="N15" s="0" t="n">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="O15" s="0" t="n">
         <f aca="false">2023-N15</f>
-        <v>7</v>
-      </c>
-      <c r="P15" s="0" t="s">
-        <v>185</v>
+        <v>10</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>222</v>
       </c>
       <c r="Q15" s="3" t="b">
         <f aca="false">IF(B15&lt;11,TRUE(),FALSE())</f>
@@ -6479,53 +6912,59 @@
       <c r="T15" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>186</v>
+      <c r="V15" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="W15" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>173</v>
+        <v>103</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>187</v>
+        <v>225</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>188</v>
+        <v>226</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="M16" s="0" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="N16" s="0" t="n">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="O16" s="0" t="n">
         <f aca="false">2023-N16</f>
-        <v>10</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>189</v>
+        <v>7</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>227</v>
       </c>
       <c r="Q16" s="3" t="b">
         <f aca="false">IF(B16&lt;11,TRUE(),FALSE())</f>
@@ -6542,53 +6981,57 @@
       <c r="T16" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V16" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="W16" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>190</v>
+      <c r="A17" s="5" t="s">
+        <v>229</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>181</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>99</v>
+        <v>179</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>192</v>
+        <v>230</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="M17" s="0" t="n">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="N17" s="0" t="n">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="O17" s="0" t="n">
         <f aca="false">2023-N17</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P17" s="0" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="Q17" s="3" t="b">
         <f aca="false">IF(B17&lt;11,TRUE(),FALSE())</f>
@@ -6605,51 +7048,57 @@
       <c r="T17" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>194</v>
+      <c r="V17" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="W17" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>233</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>66</v>
+        <v>319</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>196</v>
+        <v>234</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="K18" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="M18" s="0" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="N18" s="0" t="n">
-        <v>2015</v>
+        <v>2004</v>
       </c>
       <c r="O18" s="0" t="n">
         <f aca="false">2023-N18</f>
-        <v>8</v>
-      </c>
-      <c r="P18" s="0" t="s">
-        <v>185</v>
+        <v>19</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="Q18" s="3" t="b">
         <f aca="false">IF(B18&lt;11,TRUE(),FALSE())</f>
@@ -6666,38 +7115,50 @@
       <c r="T18" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V18" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="W18" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>197</v>
+      <c r="A19" s="5" t="s">
+        <v>238</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>319</v>
+        <v>83</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>170</v>
+        <v>175</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>38</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>199</v>
+        <v>239</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>240</v>
       </c>
       <c r="K19" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="L19" s="0" t="n">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="M19" s="0" t="n">
         <v>2019</v>
@@ -6709,8 +7170,8 @@
         <f aca="false">2023-N19</f>
         <v>19</v>
       </c>
-      <c r="P19" s="4" t="s">
-        <v>200</v>
+      <c r="P19" s="0" t="s">
+        <v>241</v>
       </c>
       <c r="Q19" s="3" t="b">
         <f aca="false">IF(B19&lt;11,TRUE(),FALSE())</f>
@@ -6724,60 +7185,67 @@
         <f aca="false">IF(B19=L19,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T19" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>83</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>175</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="K20" s="2" t="n">
+      <c r="T19" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="U19" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="W19" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>178</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="K20" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
       <c r="L20" s="0" t="n">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="M20" s="0" t="n">
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="N20" s="0" t="n">
-        <v>2004</v>
+        <v>2009</v>
       </c>
       <c r="O20" s="0" t="n">
         <f aca="false">2023-N20</f>
-        <v>19</v>
-      </c>
-      <c r="P20" s="0" t="s">
-        <v>204</v>
+        <v>14</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="Q20" s="3" t="b">
         <f aca="false">IF(B20&lt;11,TRUE(),FALSE())</f>
@@ -6789,53 +7257,57 @@
       </c>
       <c r="S20" s="3" t="b">
         <f aca="false">IF(B20=L20,TRUE(),FALSE())</f>
-        <v>0</v>
-      </c>
-      <c r="T20" s="2" t="n">
-        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U20" s="0" t="n">
+      <c r="T20" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="W20" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="K21" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="M21" s="0" t="n">
         <v>2019</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>81</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>178</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="K21" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="0" t="n">
-        <v>81</v>
-      </c>
-      <c r="M21" s="0" t="n">
-        <v>2023</v>
       </c>
       <c r="N21" s="0" t="n">
         <v>2009</v>
@@ -6844,8 +7316,8 @@
         <f aca="false">2023-N21</f>
         <v>14</v>
       </c>
-      <c r="P21" s="4" t="s">
-        <v>208</v>
+      <c r="P21" s="5" t="s">
+        <v>251</v>
       </c>
       <c r="Q21" s="3" t="b">
         <f aca="false">IF(B21&lt;11,TRUE(),FALSE())</f>
@@ -6857,58 +7329,64 @@
       </c>
       <c r="S21" s="3" t="b">
         <f aca="false">IF(B21=L21,TRUE(),FALSE())</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T21" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>209</v>
+      <c r="V21" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="W21" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>34</v>
+        <v>254</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>210</v>
+        <v>255</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>211</v>
+        <v>256</v>
+      </c>
+      <c r="K22" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="L22" s="0" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M22" s="0" t="n">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="N22" s="0" t="n">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="O22" s="0" t="n">
         <f aca="false">2023-N22</f>
-        <v>14</v>
-      </c>
-      <c r="P22" s="4" t="s">
-        <v>212</v>
+        <v>12</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>257</v>
       </c>
       <c r="Q22" s="3" t="b">
         <f aca="false">IF(B22&lt;11,TRUE(),FALSE())</f>
@@ -6925,16 +7403,22 @@
       <c r="T22" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="V22" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="W22" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>213</v>
+      <c r="A23" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>508</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>28</v>
@@ -6943,19 +7427,19 @@
         <v>174</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>214</v>
+        <v>260</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>8</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>215</v>
+        <v>261</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>216</v>
+        <v>262</v>
       </c>
       <c r="L23" s="0" t="n">
         <v>3</v>
@@ -6971,7 +7455,7 @@
         <v>15</v>
       </c>
       <c r="P23" s="0" t="s">
-        <v>217</v>
+        <v>263</v>
       </c>
       <c r="Q23" s="3" t="b">
         <f aca="false">IF(B23&lt;11,TRUE(),FALSE())</f>
@@ -6986,6 +7470,12 @@
       </c>
       <c r="T23" s="2" t="b">
         <v>0</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="W23" s="0" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -7009,6 +7499,30 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="V2" r:id="rId1" display="https://libema-open.nl/wp-content/uploads/2023/05/Bencic_Hero-Smile.webp"/>
+    <hyperlink ref="V3" r:id="rId2" display="https://libema-open.nl/wp-content/uploads/2023/05/Kudermetova_Hero-Smile.webp"/>
+    <hyperlink ref="V4" r:id="rId3" display="https://libema-open.nl/wp-content/uploads/2023/05/Samsonova_Crop.webp"/>
+    <hyperlink ref="V5" r:id="rId4" display="https://libema-open.nl/wp-content/uploads/2023/05/azarenka.webp"/>
+    <hyperlink ref="V6" r:id="rId5" display="https://libema-open.nl/wp-content/uploads/2023/05/Zheng-Torso_328120.webp"/>
+    <hyperlink ref="V7" r:id="rId6" display="https://libema-open.nl/wp-content/uploads/2023/05/Alexandrova_Hero-Smile.webp"/>
+    <hyperlink ref="V8" r:id="rId7" display="https://libema-open.nl/wp-content/uploads/2023/05/Mertens_Hero-Smile.webp"/>
+    <hyperlink ref="V9" r:id="rId8" display="https://libema-open.nl/wp-content/uploads/2023/05/Martic_Hero-Smile.webp"/>
+    <hyperlink ref="V10" r:id="rId9" display="https://libema-open.nl/wp-content/uploads/2023/05/Andreescu_crop.webp"/>
+    <hyperlink ref="V11" r:id="rId10" display="https://libema-open.nl/wp-content/uploads/2023/05/Rogers-Torso_317421.webp"/>
+    <hyperlink ref="V12" r:id="rId11" display="https://libema-open.nl/wp-content/uploads/2023/05/QcvLKQRa.webp"/>
+    <hyperlink ref="V13" r:id="rId12" display="https://libema-open.nl/wp-content/uploads/2023/05/MLBGcqtM.webp"/>
+    <hyperlink ref="V14" r:id="rId13" display="https://libema-open.nl/wp-content/uploads/2023/05/Gracheva_crop.webp"/>
+    <hyperlink ref="V15" r:id="rId14" display="https://libema-open.nl/wp-content/uploads/2023/05/Muchova_Hero-Smile.webp"/>
+    <hyperlink ref="V16" r:id="rId15" display="https://libema-open.nl/wp-content/uploads/2023/05/McNally_Crop.webp"/>
+    <hyperlink ref="V17" r:id="rId16" display="https://libema-open.nl/wp-content/uploads/2023/05/LiQQMObq.webp"/>
+    <hyperlink ref="V18" r:id="rId17" display="https://libema-open.nl/wp-content/uploads/2023/05/KxenXejL.webp"/>
+    <hyperlink ref="V19" r:id="rId18" display="https://libema-open.nl/wp-content/uploads/2023/05/SuWqgWYb.webp"/>
+    <hyperlink ref="V20" r:id="rId19" display="https://libema-open.nl/wp-content/uploads/2023/05/fNpQoEOl.webp"/>
+    <hyperlink ref="V21" r:id="rId20" display="https://libema-open.nl/wp-content/uploads/2023/05/ODTCCbpp.webp"/>
+    <hyperlink ref="V22" r:id="rId21" display="https://libema-open.nl/wp-content/uploads/2023/05/Friedsam_Crop.webp"/>
+    <hyperlink ref="V23" r:id="rId22" display="https://libema-open.nl/wp-content/uploads/2023/05/ODTCCbpp.webp"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -7037,27 +7551,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>218</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preference solicitation on one page
</commit_message>
<xml_diff>
--- a/backend/data/Competitors.xlsx
+++ b/backend/data/Competitors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Competitors-Male" sheetId="1" state="visible" r:id="rId2"/>
@@ -120,7 +120,7 @@
     <t xml:space="preserve">Funny, outspoken, Analytical, Unorthodox, Defensive Baseliner</t>
   </si>
   <si>
-    <t xml:space="preserve">Medvedev is known for his counter-punching style and excellent defensive play. His flat and deep shots, combined with his exceptional court coverage, make him a tough player to beat. He's also known for his tactical intelligence, often adjusting his game plan mid-match to exploit his opponents' weaknesses.</t>
+    <t xml:space="preserve">“Medvedev is known for his counter-punching style and excellent defensive play. His flat and deep shots, combined with his exceptional court coverage, make him a tough player to beat. He's also known for his tactical intelligence, often adjusting his game plan mid-match to exploit his opponents' weaknesses."</t>
   </si>
   <si>
     <t xml:space="preserve">Gilles Cervara</t>
@@ -147,7 +147,7 @@
     <t xml:space="preserve">Mr. Nice Guy, powerful serve, powerful forehand, Athletic, Powerful, Emotiona</t>
   </si>
   <si>
-    <t xml:space="preserve">Auger-Aliassime is an athletic player with a complete game. His serve and forehand are his biggest weapons, but he's also known for his speed and agility, allowing him to defend well. He's still maturing in terms of strategy, but his raw talent and physical attributes make him a serious threat.</t>
+    <t xml:space="preserve">“Auger-Aliassime is an athletic player with a complete game. His serve and forehand are his biggest weapons, but he's also known for his speed and agility, allowing him to defend well. He's still maturing in terms of strategy, but his raw talent and physical attributes make him a serious threat."</t>
   </si>
   <si>
     <t xml:space="preserve">Frederic Fontang, Toni Nadal</t>
@@ -165,7 +165,7 @@
     <t xml:space="preserve">Hard worker, physical, good looking, Defensive Baseliner, Mentally Tough</t>
   </si>
   <si>
-    <t xml:space="preserve"> Coric is a steady baseliner known for his mental toughness and solid groundstrokes. He's not the most aggressive player, but his consistency and ability to absorb and redirect pace can frustrate opponents. His game is characterized by strategic point construction and patience.</t>
+    <t xml:space="preserve">“Coric is a steady baseliner known for his mental toughness and solid groundstrokes. He's not the most aggressive player, but his consistency and ability to absorb and redirect pace can frustrate opponents. His game is characterized by strategic point construction and patience."</t>
   </si>
   <si>
     <t xml:space="preserve">Mate Delic</t>
@@ -183,7 +183,7 @@
     <t xml:space="preserve">Energetic, fighter, runs like crazy on every ball, Speedy, Defensive Baseliner, Counterpuncher, agile</t>
   </si>
   <si>
-    <t xml:space="preserve">De Minaur is known for his exceptional speed and relentless defense. He's a counterpuncher who excels at turning defense into offense. While he may lack the raw power of some players, his precise shot placement and ability to hit on the run often put opponents on the back foot.</t>
+    <t xml:space="preserve">“De Minaur is known for his exceptional speed and relentless defense. He's a counterpuncher who excels at turning defense into offense. While he may lack the raw power of some players, his precise shot placement and ability to hit on the run often put opponents on the back foot."</t>
   </si>
   <si>
     <t xml:space="preserve">Adolfo Gutierrez</t>
@@ -201,7 +201,7 @@
     <t xml:space="preserve">Heated when angry, hard worker, patient, consistent, strategic, groundstroke</t>
   </si>
   <si>
-    <t xml:space="preserve">Carreno Busta is a consistent player who excels on all surfaces. He doesn't possess the biggest shots, but his solid baseline game, combined with his tactical intelligence and patience, make him a difficult opponent. He's known for his ability to construct points and wait for the right moment to attack.</t>
+    <t xml:space="preserve">“Carreno Busta is a consistent player who excels on all surfaces. He doesn't possess the biggest shots, but his solid baseline game, combined with his tactical intelligence and patience, make him a difficult opponent. He's known for his ability to construct points and wait for the right moment to attack."</t>
   </si>
   <si>
     <t xml:space="preserve">Samuel Lopez, Jose Antonio Sanchez-de Luna</t>
@@ -219,31 +219,13 @@
     <t xml:space="preserve">humble, quiet, powerful, aggressive, focused, powerful serve</t>
   </si>
   <si>
-    <t xml:space="preserve">Cilic's game is centered around his powerful serve and aggressive groundstrokes. He looks to dictate play from the baseline and finish points at the net when possible. His aggressive game style has led him to success, including a Grand Slam title at the US Open in 2014.</t>
+    <t xml:space="preserve">“Cilic's game is centered around his powerful serve and aggressive groundstrokes. He looks to dictate play from the baseline and finish points at the net when possible. His aggressive game style has led him to success, including a Grand Slam title at the US Open in 2014."</t>
   </si>
   <si>
     <t xml:space="preserve">Ivan Cinkus, Vilim Visak</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://libema-open.nl/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/wp-content/uploads/2023/05/cilic-full-2022-may.png</t>
-    </r>
+    <t xml:space="preserve">https://libema-open.nl//wp-content/uploads/2023/05/cilic-full-2022-may.png</t>
   </si>
   <si>
     <t xml:space="preserve">Roberto Bautista Agut</t>
@@ -252,31 +234,13 @@
     <t xml:space="preserve">Feisty, fighter, focused, endurance, calm</t>
   </si>
   <si>
-    <t xml:space="preserve">Bautista Agut is a grinder on the court. He's not the most powerful player, but his consistency from the baseline, excellent footwork, and mental toughness make him a tough opponent. He's known for his ability to sustain long rallies and wear down opponents.</t>
+    <t xml:space="preserve">“Bautista Agut is a grinder on the court. He's not the most powerful player, but his consistency from the baseline, excellent footwork, and mental toughness make him a tough opponent. He's known for his ability to sustain long rallies and wear down opponents."</t>
   </si>
   <si>
     <t xml:space="preserve">Daniel Gimeno-Traver, Felix Mantilla</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://libema-open.nl/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">wp-content/uploads/2023/05/bautista-agut-full-2022-may.png</t>
-    </r>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/bautista-agut-full-2022-may.png</t>
   </si>
   <si>
     <t xml:space="preserve">Botic van de Zandschulp</t>
@@ -291,31 +255,13 @@
     <t xml:space="preserve">Local hero, shy, quiet, aggressive, fighting spirit</t>
   </si>
   <si>
-    <t xml:space="preserve">An aggressive player with a solid serve and forehand. He is known for his fighting spirit on court.</t>
+    <t xml:space="preserve">“An aggressive player with a solid serve and forehand. He is known for his fighting spirit on court."</t>
   </si>
   <si>
     <t xml:space="preserve">Peter Lucassen</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://libema-open.nl/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">wp-content/uploads/2023/05/van-de-zandschulp-full-2022-may.png</t>
-    </r>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/van-de-zandschulp-full-2022-may.png</t>
   </si>
   <si>
     <t xml:space="preserve">Milos Raonic</t>
@@ -327,7 +273,7 @@
     <t xml:space="preserve">Big serve, Mr. Nice Guy, powerful serve, aggressive, composed</t>
   </si>
   <si>
-    <t xml:space="preserve">Raonic's game is built around his powerful serve, which is one of the best in the men's game. He also has powerful groundstrokes and seeks to play aggressively, often looking to finish points at the net. He's worked to improve his mobility and baseline game throughout his career.</t>
+    <t xml:space="preserve">“Raonic's game is built around his powerful serve, which is one of the best in the men's game. He also has powerful groundstrokes and seeks to play aggressively, often looking to finish points at the net. He's worked to improve his mobility and baseline game throughout his career."</t>
   </si>
   <si>
     <t xml:space="preserve">Mario Tudor</t>
@@ -345,7 +291,7 @@
     <t xml:space="preserve">Outspoken, interactive, local hero, powerful serve</t>
   </si>
   <si>
-    <t xml:space="preserve">Known for his powerful serve and aggressive baseline play. </t>
+    <t xml:space="preserve">“Known for his powerful serve and aggressive baseline play. "</t>
   </si>
   <si>
     <t xml:space="preserve">Kristof Vliegen</t>
@@ -363,7 +309,7 @@
     <t xml:space="preserve">consistent, fighting spirit, groundstroke</t>
   </si>
   <si>
-    <t xml:space="preserve">Kecmanovic is a steady baseliner with solid groundstrokes from both wings. He has a well-rounded game, with no significant weaknesses, and he's known for his fighting spirit and ability to maintain a high level of play under pressure.</t>
+    <t xml:space="preserve">“Kecmanovic is a steady baseliner with solid groundstrokes from both wings. He has a well-rounded game, with no significant weaknesses, and he's known for his fighting spirit and ability to maintain a high level of play under pressure."</t>
   </si>
   <si>
     <t xml:space="preserve">Wayne Black, Ivan Cinkus</t>
@@ -378,7 +324,7 @@
     <t xml:space="preserve">Emotional, funny, interactive, patient, clay-court specialist</t>
   </si>
   <si>
-    <t xml:space="preserve">A Spanish tennis player, Miralles is known for his clay-court skills, which are typical of many Spanish players. His game is characterised by heavy topspin from the baseline, particularly on the forehand side, and a patient approach, often waiting for his opponent to make errors rather than going for outright winners.</t>
+    <t xml:space="preserve">“A Spanish tennis player, Miralles is known for his clay-court skills, which are typical of many Spanish players. His game is characterised by heavy topspin from the baseline, particularly on the forehand side, and a patient approach, often waiting for his opponent to make errors rather than going for outright winners."</t>
   </si>
   <si>
     <t xml:space="preserve">Samuel Ribeiro</t>
@@ -396,7 +342,7 @@
     <t xml:space="preserve">Focused, shy, quiet, energetic</t>
   </si>
   <si>
-    <t xml:space="preserve">A player with an aggressive playing style, Cressy is notable for his serve-and-volley tactics, a relatively rare strategy in modern tennis. He possesses a powerful serve and isn't afraid to approach the net, looking to finish points quickly.</t>
+    <t xml:space="preserve">“A player with an aggressive playing style, Cressy is notable for his serve-and-volley tactics, a relatively rare strategy in modern tennis. He possesses a powerful serve and isn't afraid to approach the net, looking to finish points quickly."</t>
   </si>
   <si>
     <t xml:space="preserve">Alexandre Sidorenko, Juanjo Climent, Andrew Mawire </t>
@@ -414,7 +360,7 @@
     <t xml:space="preserve">Focused, cool, consistent</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ruusuvuori has a solid baseline game, powerful from both wings, with a particular strength in his backhand. He's also known for his fighting spirit and mental toughness on the court. Off the court, he has diverse interests from music to hockey.</t>
+    <t xml:space="preserve">“ Ruusuvuori has a solid baseline game, powerful from both wings, with a particular strength in his backhand. He's also known for his fighting spirit and mental toughness on the court. Off the court, he has diverse interests from music to hockey."</t>
   </si>
   <si>
     <t xml:space="preserve">Federico Ricci</t>
@@ -438,7 +384,7 @@
     <t xml:space="preserve">Creative, focused, quiet, precise, groundstroke, unorthodox</t>
   </si>
   <si>
-    <t xml:space="preserve">Mannarino is known for his unorthodox playing style. He has a flat groundstroke and an excellent sense of timing, often disrupting opponents with unpredictable shot selection. He is also known for his excellent footwork and defensive skills.</t>
+    <t xml:space="preserve">“Mannarino is known for his unorthodox playing style. He has a flat groundstroke and an excellent sense of timing, often disrupting opponents with unpredictable shot selection. He is also known for his excellent footwork and defensive skills."</t>
   </si>
   <si>
     <t xml:space="preserve">Erwann Tortuyaux</t>
@@ -453,7 +399,7 @@
     <t xml:space="preserve">Perfectionist, well-schooled, composed</t>
   </si>
   <si>
-    <t xml:space="preserve">Nakashima has a powerful baseline game, especially his backhand, and is known for his tactical intelligence and composure on court. His serve is also a significant weapon, allowing him to control many points from the onset.</t>
+    <t xml:space="preserve">“Nakashima has a powerful baseline game, especially his backhand, and is known for his tactical intelligence and composure on court. His serve is also a significant weapon, allowing him to control many points from the onset."</t>
   </si>
   <si>
     <t xml:space="preserve">Edwardo Infantino</t>
@@ -471,7 +417,7 @@
     <t xml:space="preserve">Showman, outspoken, interactive, unpredictable, entertaining</t>
   </si>
   <si>
-    <t xml:space="preserve">Bublik is known for his unpredictable and often flashy style of play. He has a powerful serve and isn't afraid to use underarm serves to catch his opponents off guard. He also frequently employs drop shots and has a strong net game.</t>
+    <t xml:space="preserve">“Bublik is known for his unpredictable and often flashy style of play. He has a powerful serve and isn't afraid to use underarm serves to catch his opponents off guard. He also frequently employs drop shots and has a strong net game."</t>
   </si>
   <si>
     <t xml:space="preserve">Artem Suprunov</t>
@@ -486,7 +432,7 @@
     <t xml:space="preserve">aggressive, focused, powerful serve, powerful forehand, quiet</t>
   </si>
   <si>
-    <t xml:space="preserve">A left-handed player, Humbert is known for his aggressive all-court game. He has a strong serve and a potent one-handed backhand, and he likes to take control of points early. He's also known for his ability to vary the pace and spin of his shots, often keeping opponents off balance.</t>
+    <t xml:space="preserve">“A left-handed player, Humbert is known for his aggressive all-court game. He has a strong serve and a potent one-handed backhand, and he likes to take control of points early. He's also known for his ability to vary the pace and spin of his shots, often keeping opponents off balance."</t>
   </si>
   <si>
     <t xml:space="preserve">Jeremy Chardy</t>
@@ -504,7 +450,7 @@
     <t xml:space="preserve">Big serve, local hero, speedy, agile, fighting spirit</t>
   </si>
   <si>
-    <t xml:space="preserve">Ymer is a steady baseline player with a solid two-handed backhand. He's known for his speed and athleticism on the court, often engaging opponents in long rallies and outlasting them with his physicality and endurance.</t>
+    <t xml:space="preserve">“Ymer is a steady baseline player with a solid two-handed backhand. He's known for his speed and athleticism on the court, often engaging opponents in long rallies and outlasting them with his physicality and endurance."</t>
   </si>
   <si>
     <t xml:space="preserve">Daniel Berta</t>
@@ -522,7 +468,7 @@
     <t xml:space="preserve">powerful serve, powerful groundstroke, aggressive</t>
   </si>
   <si>
-    <t xml:space="preserve"> van Rijthoven has a game that is characterized by a strong serve and an aggressive baseline play. He prefers hard courts and isn't afraid to approach the net, often looking to finish points quickly.</t>
+    <t xml:space="preserve">“van Rijthoven has a game that is characterized by a strong serve and an aggressive baseline play. He prefers hard courts and isn't afraid to approach the net, often looking to finish points quickly."</t>
   </si>
   <si>
     <t xml:space="preserve">Igor Sijsling</t>
@@ -540,7 +486,7 @@
     <t xml:space="preserve">Olympian, groundstroke, tactical, defensive, serve, footwork</t>
   </si>
   <si>
-    <t xml:space="preserve">Bencic possesses a versatile game marked by excellent court coverage and an ability to change direction of the ball with ease. Her smart tactical sense allows her to construct points effectively, often outmaneuvering her opponents with precise shot placement.</t>
+    <t xml:space="preserve">“Bencic possesses a versatile game marked by excellent court coverage and an ability to change direction of the ball with ease. Her smart tactical sense allows her to construct points effectively, often outmaneuvering her opponents with precise shot placement."</t>
   </si>
   <si>
     <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Bencic_Hero-Smile.webp</t>
@@ -555,7 +501,7 @@
     <t xml:space="preserve">serve, forehand, net game, backhand</t>
   </si>
   <si>
-    <t xml:space="preserve">Kudermetova has a strong baseline game, characterized by powerful groundstrokes. She has an aggressive style of play, often looking to dictate points with her strong serve and forehand.</t>
+    <t xml:space="preserve">“Kudermetova has a strong baseline game, characterized by powerful groundstrokes. She has an aggressive style of play, often looking to dictate points with her strong serve and forehand."</t>
   </si>
   <si>
     <t xml:space="preserve">Sergey Demekhine, Vladimir Platenik</t>
@@ -570,7 +516,7 @@
     <t xml:space="preserve">Long games, groundstrokes, aggressive, serve, consistent, mental toughness</t>
   </si>
   <si>
-    <t xml:space="preserve">Samsonova is known for her aggressive game. She has powerful groundstrokes from both wings and a strong serve, which allows her to dictate play and keep opponents on the back foot.</t>
+    <t xml:space="preserve">“Samsonova is known for her aggressive game. She has powerful groundstrokes from both wings and a strong serve, which allows her to dictate play and keep opponents on the back foot."</t>
   </si>
   <si>
     <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Samsonova_Crop.webp</t>
@@ -582,7 +528,7 @@
     <t xml:space="preserve">Outspoken, fighter, showman, Consistent, movement, groundstrokes, serve, competitive</t>
   </si>
   <si>
-    <t xml:space="preserve">A former world No. 1, Azarenka's game is characterized by her powerful baseline play and strong return of serve, often taking the ball early and redirecting with pace. She's also noted for her mental toughness and competitive spirit on court.</t>
+    <t xml:space="preserve">“A former world No. 1, Azarenka's game is characterized by her powerful baseline play and strong return of serve, often taking the ball early and redirecting with pace. She's also noted for her mental toughness and competitive spirit on court."</t>
   </si>
   <si>
     <t xml:space="preserve">Maxime Tchoutakian</t>
@@ -600,7 +546,7 @@
     <t xml:space="preserve">Talented, Versatile, strong groundstrokes, powerful serve, aggressive, net play</t>
   </si>
   <si>
-    <t xml:space="preserve">Zheng is a young player known for her aggressive game style, with a powerful serve and strong groundstrokes. She often looks to dictate the play and isn't afraid to go for winners.</t>
+    <t xml:space="preserve">“Zheng is a young player known for her aggressive game style, with a powerful serve and strong groundstrokes. She often looks to dictate the play and isn't afraid to go for winners."</t>
   </si>
   <si>
     <t xml:space="preserve">Pedro Riba Madrid</t>
@@ -615,7 +561,7 @@
     <t xml:space="preserve">Quiet, serve, aggressive, forehand, consistent, mental toughness</t>
   </si>
   <si>
-    <t xml:space="preserve">Alexandrova is known for her aggressive baseline game. She possesses a powerful serve and forehand, often looking to finish points quickly rather than engage in extended rallies.</t>
+    <t xml:space="preserve">“Alexandrova is known for her aggressive baseline game. She possesses a powerful serve and forehand, often looking to finish points quickly rather than engage in extended rallies."</t>
   </si>
   <si>
     <t xml:space="preserve">Evgeny Alexandrova</t>
@@ -633,7 +579,7 @@
     <t xml:space="preserve">Lovely, respectful, interactive, Consistent, footwork, groundstrokes, serve, defensive</t>
   </si>
   <si>
-    <t xml:space="preserve">Mertens has a well-rounded game, marked by solid groundstrokes, good court coverage and tactical intelligence. Her versatile game allows her to adapt to different playing styles and court surfaces.</t>
+    <t xml:space="preserve">“Mertens has a well-rounded game, marked by solid groundstrokes, good court coverage and tactical intelligence. Her versatile game allows her to adapt to different playing styles and court surfaces."</t>
   </si>
   <si>
     <t xml:space="preserve">Alexander Kneepkens</t>
@@ -648,7 +594,7 @@
     <t xml:space="preserve">Well-trained, groundstrokes, tactical, serve, net play, defensive</t>
   </si>
   <si>
-    <t xml:space="preserve">Martic is a strategic player known for her variety, often mixing up pace and spin to disrupt her opponent's rhythm. She has a strong serve and is particularly effective at the net, with good volleying skills.</t>
+    <t xml:space="preserve">“Martic is a strategic player known for her variety, often mixing up pace and spin to disrupt her opponent's rhythm. She has a strong serve and is particularly effective at the net, with good volleying skills."</t>
   </si>
   <si>
     <t xml:space="preserve">Michael Geserer</t>
@@ -663,7 +609,7 @@
     <t xml:space="preserve">Talented, entertaining, fighter, Versatile, groundstrokes, aggressive, serve, competitive</t>
   </si>
   <si>
-    <t xml:space="preserve">Andreescu's game is characterized by its variety and power. She has strong groundstrokes, a potent serve, and isn't afraid to come forward and finish points at the net. She also uses a variety of spins and paces to disrupt her opponents.</t>
+    <t xml:space="preserve">“Andreescu's game is characterized by its variety and power. She has strong groundstrokes, a potent serve, and isn't afraid to come forward and finish points at the net. She also uses a variety of spins and paces to disrupt her opponents."</t>
   </si>
   <si>
     <t xml:space="preserve">Christphe Lambert</t>
@@ -678,7 +624,7 @@
     <t xml:space="preserve">serve, groundstrokes, aggressive, net play, mental toughness</t>
   </si>
   <si>
-    <t xml:space="preserve">Rogers is known for her powerful serve and aggressive baseline play. She has a strong forehand and isn't afraid to attack and dictate the play, often seeking to finish points quickly.</t>
+    <t xml:space="preserve">“Rogers is known for her powerful serve and aggressive baseline play. She has a strong forehand and isn't afraid to attack and dictate the play, often seeking to finish points quickly."</t>
   </si>
   <si>
     <t xml:space="preserve">Piotr Sierzputowski</t>
@@ -696,7 +642,7 @@
     <t xml:space="preserve">Positive, runs a lot, Consistent, groundstrokes, movement, defensive, serve</t>
   </si>
   <si>
-    <t xml:space="preserve">Bouzkova is known for her consistent baseline game and good court coverage. She has solid groundstrokes and a good defensive game, often forcing opponents into errors.</t>
+    <t xml:space="preserve">“Bouzkova is known for her consistent baseline game and good court coverage. She has solid groundstrokes and a good defensive game, often forcing opponents into errors."</t>
   </si>
   <si>
     <t xml:space="preserve">Cristian Requeni, Milan Bouzek</t>
@@ -714,7 +660,7 @@
     <t xml:space="preserve">Versatile, groundstrokes, serve, consistency, tactical</t>
   </si>
   <si>
-    <t xml:space="preserve">Sasnovich is a consistent player with solid groundstrokes from both wings. She often plays a patient game from the baseline, waiting for her opponents to make errors.</t>
+    <t xml:space="preserve">“Sasnovich is a consistent player with solid groundstrokes from both wings. She often plays a patient game from the baseline, waiting for her opponents to make errors."</t>
   </si>
   <si>
     <t xml:space="preserve">Dzmitry Klimenko</t>
@@ -729,7 +675,7 @@
     <t xml:space="preserve">serve, aggressive, groundstrokes, consistent, footwork</t>
   </si>
   <si>
-    <t xml:space="preserve">Gracheva's game is characterized by her solid baseline play and consistent groundstrokes. She has a patient approach to her game, often engaging in long rallies and waiting for her opponent to make errors.</t>
+    <t xml:space="preserve">“Gracheva's game is characterized by her solid baseline play and consistent groundstrokes. She has a patient approach to her game, often engaging in long rallies and waiting for her opponent to make errors."</t>
   </si>
   <si>
     <t xml:space="preserve">Xavier Pujo</t>
@@ -744,7 +690,7 @@
     <t xml:space="preserve">Versatile, serve, groundstrokes, aggressive, net play</t>
   </si>
   <si>
-    <t xml:space="preserve">Muchova has a versatile game, with a good mix of power and finesse. She often employs a variety of shots, including slices and drop shots, to disrupt her opponent's rhythm.</t>
+    <t xml:space="preserve">“Muchova has a versatile game, with a good mix of power and finesse. She often employs a variety of shots, including slices and drop shots, to disrupt her opponent's rhythm."</t>
   </si>
   <si>
     <t xml:space="preserve">David Kotyza</t>
@@ -759,10 +705,10 @@
     <t xml:space="preserve">Aggressive, strong serve, versatile, doubles strength, net game</t>
   </si>
   <si>
-    <t xml:space="preserve">Known for her aggressive style and strong serve, Caty McNally is a versatile player who can excel on various surfaces. She's made a name for herself in doubles, often partnering with fellow American Coco Gauff, and has started to break through in singles as well. With a potent one-two punch of a big serve followed by a heavy groundstroke, McNally can quickly take control of points. She also possesses a rare weapon in the women's game: a strong net game, thanks to her doubles expertise.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kevin O’Neill</t>
+    <t xml:space="preserve">“Known for her aggressive style and strong serve, Caty McNally is a versatile player who can excel on various surfaces. She's made a name for herself in doubles, often partnering with fellow American Coco Gauff, and has started to break through in singles as well. With a potent one-two punch of a big serve followed by a heavy groundstroke, McNally can quickly take control of points. She also possesses a rare weapon in the women's game: a strong net game, thanks to her doubles expertise.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Kevin O’Neill”</t>
   </si>
   <si>
     <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/McNally_Crop.webp</t>
@@ -774,7 +720,7 @@
     <t xml:space="preserve">Aggressive, all-court player, powerful groundstrokes</t>
   </si>
   <si>
-    <t xml:space="preserve">Anna Blinkova is a solid all-court player known for her powerful groundstrokes. Her aggressive style of play often sees her taking the ball on the rise and aiming for the lines. Blinkova has shown that she can compete at the top level and has recorded victories against higher-ranked opponents. Her ability to generate power from both wings and her willingness to attack and dictate play are key elements of her game.</t>
+    <t xml:space="preserve">“Anna Blinkova is a solid all-court player known for her powerful groundstrokes. Her aggressive style of play often sees her taking the ball on the rise and aiming for the lines. Blinkova has shown that she can compete at the top level and has recorded victories against higher-ranked opponents. Her ability to generate power from both wings and her willingness to attack and dictate play are key elements of her game.”</t>
   </si>
   <si>
     <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/LiQQMObq.webp</t>
@@ -786,7 +732,7 @@
     <t xml:space="preserve">Consistent, tactical, changes pace, court awareness</t>
   </si>
   <si>
-    <t xml:space="preserve">Evgeniya Rodina is a seasoned player with a well-rounded game. Known for her consistency and tactical intelligence, she can change up the pace and spin of her shots to disrupt her opponent's rhythm. While not the most powerful player on tour, Rodina uses her court awareness and shot selection effectively to construct points.</t>
+    <t xml:space="preserve">“Evgeniya Rodina is a seasoned player with a well-rounded game. Known for her consistency and tactical intelligence, she can change up the pace and spin of her shots to disrupt her opponent's rhythm. While not the most powerful player on tour, Rodina uses her court awareness and shot selection effectively to construct points."</t>
   </si>
   <si>
     <t xml:space="preserve">Oxana Mishikova</t>
@@ -801,7 +747,7 @@
     <t xml:space="preserve">Aggressive, positive, powerful groundstrokes, strong serve, net play, tough competitor</t>
   </si>
   <si>
-    <t xml:space="preserve">Alison Riske-Amritraj is known for her aggressive baseline play and powerful groundstrokes. Her strengths include a strong serve and a particularly effective backhand. She also has a knack for coming to the net, showcasing her versatile skill set. Over the years, Riske-Amritraj has developed a reputation for being a tough competitor, often playing her best tennis in tight situations.</t>
+    <t xml:space="preserve">“Alison Riske-Amritraj is known for her aggressive baseline play and powerful groundstrokes. Her strengths include a strong serve and a particularly effective backhand. She also has a knack for coming to the net, showcasing her versatile skill set. Over the years, Riske-Amritraj has developed a reputation for being a tough competitor, often playing her best tennis in tight situations."</t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Gutteridge</t>
@@ -816,7 +762,7 @@
     <t xml:space="preserve">Left-handed, powerful serve, topspin forehand, aggressive, high-risk</t>
   </si>
   <si>
-    <t xml:space="preserve">Ysaline Bonaventure is a left-handed player known for her powerful serve and heavy topspin forehand. Her game is characterized by aggressive shot-making and the ability to generate pace from both wings. While she can be erratic at times, her high-risk style of play can be very effective when she's in form.</t>
+    <t xml:space="preserve">“Ysaline Bonaventure is a left-handed player known for her powerful serve and heavy topspin forehand. Her game is characterized by aggressive shot-making and the ability to generate pace from both wings. While she can be erratic at times, her high-risk style of play can be very effective when she's in form."</t>
   </si>
   <si>
     <t xml:space="preserve">Hugo Guerriero</t>
@@ -831,7 +777,7 @@
     <t xml:space="preserve">Baseline player, consistent, strong groundstrokes, defensive, counterpunching, fighting spirit</t>
   </si>
   <si>
-    <t xml:space="preserve">Rebecca Peterson is a solid baseline player with a consistent game. She uses her strong groundstrokes to construct points and can change direction of the ball effectively. Peterson also has a good defensive game, often turning defense into offense with her counterpunching ability. She's known for her fighting spirit on the court, often grinding out tough matches.</t>
+    <t xml:space="preserve">“Rebecca Peterson is a solid baseline player with a consistent game. She uses her strong groundstrokes to construct points and can change direction of the ball effectively. Peterson also has a good defensive game, often turning defense into offense with her counterpunching ability. She's known for her fighting spirit on the court, often grinding out tough matches."</t>
   </si>
   <si>
     <t xml:space="preserve">Mart Peterson</t>
@@ -849,7 +795,7 @@
     <t xml:space="preserve">groundstrokes, aggressive</t>
   </si>
   <si>
-    <t xml:space="preserve">Anna-Lena Friedsam is an aggressive baseliner who relies on her powerful groundstrokes to dictate play. She looks to take control of the rallies by hitting aggressive shots and going for winners. At the same time, she has the ability to defend and counter-punch effectively, adjusting her game according to the situation.</t>
+    <t xml:space="preserve">“Anna-Lena Friedsam is an aggressive baseliner who relies on her powerful groundstrokes to dictate play. She looks to take control of the rallies by hitting aggressive shots and going for winners. At the same time, she has the ability to defend and counter-punch effectively, adjusting her game according to the situation."</t>
   </si>
   <si>
     <t xml:space="preserve">Patrice Hopfe</t>
@@ -867,7 +813,7 @@
     <t xml:space="preserve">Consistent, excellent movement, defensive skills, solid groundstrokes, mental toughness, competitive spirit</t>
   </si>
   <si>
-    <t xml:space="preserve">Elina Svitolina is one of the most consistent players on the WTA Tour, known for her excellent movement, strong defensive skills, and the ability to turn defense into offense. Her game is based around her solid groundstrokes and her ability to move her opponents around the court. Svitolina is also known for her mental toughness and strong competitive spirit, often elevating her game in important moments.</t>
+    <t xml:space="preserve">“Elina Svitolina is one of the most consistent players on the WTA Tour, known for her excellent movement, strong defensive skills, and the ability to turn defense into offense. Her game is based around her solid groundstrokes and her ability to move her opponents around the court. Svitolina is also known for her mental toughness and strong competitive spirit, often elevating her game in important moments."</t>
   </si>
   <si>
     <t xml:space="preserve">Raemon Sluiter</t>
@@ -1086,15 +1032,15 @@
   </sheetPr>
   <dimension ref="A1:Y1021"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y2" activeCellId="0" sqref="Y2"/>
+      <selection pane="bottomRight" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.45"/>
@@ -1733,7 +1679,8 @@
         <f aca="false">IF(B8=M8,"All time high","")</f>
         <v/>
       </c>
-      <c r="V8" s="2" t="b">
+      <c r="V8" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="W8" s="0" t="n">
@@ -5837,9 +5784,9 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="X6" r:id="rId1" display="https://libema-open.nl/wp-content/uploads/2023/05/carreno-busta-full-2022-may.png"/>
-    <hyperlink ref="X7" r:id="rId2" display="https://libema-open.nl/"/>
-    <hyperlink ref="X8" r:id="rId3" display="https://libema-open.nl/"/>
-    <hyperlink ref="X9" r:id="rId4" display="https://libema-open.nl/"/>
+    <hyperlink ref="X7" r:id="rId2" display="https://libema-open.nl//wp-content/uploads/2023/05/cilic-full-2022-may.png"/>
+    <hyperlink ref="X8" r:id="rId3" display="https://libema-open.nl/wp-content/uploads/2023/05/bautista-agut-full-2022-may.png"/>
+    <hyperlink ref="X9" r:id="rId4" display="https://libema-open.nl/wp-content/uploads/2023/05/van-de-zandschulp-full-2022-may.png"/>
     <hyperlink ref="X10" r:id="rId5" display="https://libema-open.nl/wp-content/uploads/2023/05/raonic_full_ao20.png"/>
     <hyperlink ref="X11" r:id="rId6" display="https://libema-open.nl/wp-content/uploads/2023/05/griekspoor-full-2022-may.png"/>
     <hyperlink ref="X12" r:id="rId7" display="https://libema-open.nl/wp-content/uploads/2023/05/kecmanovic_full_2022_october-1.png"/>
@@ -5870,15 +5817,15 @@
   </sheetPr>
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V3" activeCellId="0" sqref="V3"/>
+      <selection pane="bottomRight" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.34"/>
@@ -6016,6 +5963,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V2" s="4" t="s">
@@ -6082,6 +6030,7 @@
         <v>0</v>
       </c>
       <c r="T3" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V3" s="4" t="s">
@@ -6145,6 +6094,7 @@
         <v>0</v>
       </c>
       <c r="T4" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V4" s="4" t="s">
@@ -6215,6 +6165,7 @@
         <v>0</v>
       </c>
       <c r="T5" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V5" s="4" t="s">
@@ -6281,6 +6232,7 @@
         <v>1</v>
       </c>
       <c r="T6" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V6" s="4" t="s">
@@ -6424,6 +6376,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V8" s="4" t="s">
@@ -6497,6 +6450,7 @@
         <v>0</v>
       </c>
       <c r="T9" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V9" s="4" t="s">
@@ -6566,6 +6520,7 @@
         <v>0</v>
       </c>
       <c r="T10" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V10" s="4" t="s">
@@ -6639,6 +6594,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V11" s="4" t="s">
@@ -6708,6 +6664,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V12" s="4" t="s">
@@ -6778,6 +6735,7 @@
         <v>0</v>
       </c>
       <c r="T13" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V13" s="4" t="s">
@@ -6841,6 +6799,7 @@
         <v>0</v>
       </c>
       <c r="T14" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V14" s="4" t="s">
@@ -6910,6 +6869,7 @@
         <v>0</v>
       </c>
       <c r="T15" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V15" s="4" t="s">
@@ -6919,7 +6879,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>224</v>
       </c>
@@ -6979,6 +6939,7 @@
         <v>0</v>
       </c>
       <c r="T16" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V16" s="4" t="s">
@@ -7046,6 +7007,7 @@
         <v>0</v>
       </c>
       <c r="T17" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V17" s="4" t="s">
@@ -7113,6 +7075,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V18" s="4" t="s">
@@ -7260,6 +7223,7 @@
         <v>1</v>
       </c>
       <c r="T20" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V20" s="4" t="s">
@@ -7269,7 +7233,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
         <v>248</v>
       </c>
@@ -7301,6 +7265,7 @@
         <v>250</v>
       </c>
       <c r="K21" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L21" s="0" t="n">
@@ -7332,6 +7297,7 @@
         <v>0</v>
       </c>
       <c r="T21" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V21" s="4" t="s">
@@ -7370,6 +7336,7 @@
         <v>256</v>
       </c>
       <c r="K22" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L22" s="0" t="n">
@@ -7401,6 +7368,7 @@
         <v>0</v>
       </c>
       <c r="T22" s="3" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V22" s="4" t="s">
@@ -7465,10 +7433,12 @@
         <f aca="false">IF(L23&lt;11,TRUE(),FALSE())</f>
         <v>1</v>
       </c>
-      <c r="S23" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T23" s="2" t="b">
+      <c r="S23" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="T23" s="2" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="V23" s="4" t="s">
@@ -7544,7 +7514,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.45"/>
   </cols>

</xml_diff>

<commit_message>
Fix nan values personal data
</commit_message>
<xml_diff>
--- a/backend/data/Competitors.xlsx
+++ b/backend/data/Competitors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Competitors-Male" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="268">
   <si>
     <t xml:space="preserve">Player</t>
   </si>
@@ -120,7 +120,7 @@
     <t xml:space="preserve">Funny, outspoken, Analytical, Unorthodox, Defensive Baseliner</t>
   </si>
   <si>
-    <t xml:space="preserve">“Medvedev is known for his counter-punching style and excellent defensive play. His flat and deep shots, combined with his exceptional court coverage, make him a tough player to beat. He's also known for his tactical intelligence, often adjusting his game plan mid-match to exploit his opponents' weaknesses."</t>
+    <t xml:space="preserve">Medvedev is known for his counter-punching style and excellent defensive play. His flat and deep shots, combined with his exceptional court coverage, make him a tough player to beat. He's also known for his tactical intelligence, often adjusting his game plan mid-match to exploit his opponents' weaknesses.</t>
   </si>
   <si>
     <t xml:space="preserve">Gilles Cervara</t>
@@ -147,7 +147,7 @@
     <t xml:space="preserve">Mr. Nice Guy, powerful serve, powerful forehand, Athletic, Powerful, Emotiona</t>
   </si>
   <si>
-    <t xml:space="preserve">“Auger-Aliassime is an athletic player with a complete game. His serve and forehand are his biggest weapons, but he's also known for his speed and agility, allowing him to defend well. He's still maturing in terms of strategy, but his raw talent and physical attributes make him a serious threat."</t>
+    <t xml:space="preserve">Auger-Aliassime is an athletic player with a complete game. His serve and forehand are his biggest weapons, but he's also known for his speed and agility, allowing him to defend well. He's still maturing in terms of strategy, but his raw talent and physical attributes make him a serious threat.</t>
   </si>
   <si>
     <t xml:space="preserve">Frederic Fontang, Toni Nadal</t>
@@ -165,7 +165,7 @@
     <t xml:space="preserve">Hard worker, physical, good looking, Defensive Baseliner, Mentally Tough</t>
   </si>
   <si>
-    <t xml:space="preserve">“Coric is a steady baseliner known for his mental toughness and solid groundstrokes. He's not the most aggressive player, but his consistency and ability to absorb and redirect pace can frustrate opponents. His game is characterized by strategic point construction and patience."</t>
+    <t xml:space="preserve">Coric is a steady baseliner known for his mental toughness and solid groundstrokes. He's not the most aggressive player, but his consistency and ability to absorb and redirect pace can frustrate opponents. His game is characterized by strategic point construction and patience.</t>
   </si>
   <si>
     <t xml:space="preserve">Mate Delic</t>
@@ -183,7 +183,7 @@
     <t xml:space="preserve">Energetic, fighter, runs like crazy on every ball, Speedy, Defensive Baseliner, Counterpuncher, agile</t>
   </si>
   <si>
-    <t xml:space="preserve">“De Minaur is known for his exceptional speed and relentless defense. He's a counterpuncher who excels at turning defense into offense. While he may lack the raw power of some players, his precise shot placement and ability to hit on the run often put opponents on the back foot."</t>
+    <t xml:space="preserve">De Minaur is known for his exceptional speed and relentless defense. He's a counterpuncher who excels at turning defense into offense. While he may lack the raw power of some players, his precise shot placement and ability to hit on the run often put opponents on the back foot.</t>
   </si>
   <si>
     <t xml:space="preserve">Adolfo Gutierrez</t>
@@ -201,7 +201,7 @@
     <t xml:space="preserve">Heated when angry, hard worker, patient, consistent, strategic, groundstroke</t>
   </si>
   <si>
-    <t xml:space="preserve">“Carreno Busta is a consistent player who excels on all surfaces. He doesn't possess the biggest shots, but his solid baseline game, combined with his tactical intelligence and patience, make him a difficult opponent. He's known for his ability to construct points and wait for the right moment to attack."</t>
+    <t xml:space="preserve">Carreno Busta is a consistent player who excels on all surfaces. He doesn't possess the biggest shots, but his solid baseline game, combined with his tactical intelligence and patience, make him a difficult opponent. He's known for his ability to construct points and wait for the right moment to attack.</t>
   </si>
   <si>
     <t xml:space="preserve">Samuel Lopez, Jose Antonio Sanchez-de Luna</t>
@@ -219,7 +219,7 @@
     <t xml:space="preserve">humble, quiet, powerful, aggressive, focused, powerful serve</t>
   </si>
   <si>
-    <t xml:space="preserve">“Cilic's game is centered around his powerful serve and aggressive groundstrokes. He looks to dictate play from the baseline and finish points at the net when possible. His aggressive game style has led him to success, including a Grand Slam title at the US Open in 2014."</t>
+    <t xml:space="preserve">Cilic's game is centered around his powerful serve and aggressive groundstrokes. He looks to dictate play from the baseline and finish points at the net when possible. His aggressive game style has led him to success, including a Grand Slam title at the US Open in 2014.</t>
   </si>
   <si>
     <t xml:space="preserve">Ivan Cinkus, Vilim Visak</t>
@@ -234,7 +234,7 @@
     <t xml:space="preserve">Feisty, fighter, focused, endurance, calm</t>
   </si>
   <si>
-    <t xml:space="preserve">“Bautista Agut is a grinder on the court. He's not the most powerful player, but his consistency from the baseline, excellent footwork, and mental toughness make him a tough opponent. He's known for his ability to sustain long rallies and wear down opponents."</t>
+    <t xml:space="preserve">Bautista Agut is a grinder on the court. He's not the most powerful player, but his consistency from the baseline, excellent footwork, and mental toughness make him a tough opponent. He's known for his ability to sustain long rallies and wear down opponents.</t>
   </si>
   <si>
     <t xml:space="preserve">Daniel Gimeno-Traver, Felix Mantilla</t>
@@ -255,7 +255,7 @@
     <t xml:space="preserve">Local hero, shy, quiet, aggressive, fighting spirit</t>
   </si>
   <si>
-    <t xml:space="preserve">“An aggressive player with a solid serve and forehand. He is known for his fighting spirit on court."</t>
+    <t xml:space="preserve">An aggressive player with a solid serve and forehand. He is known for his fighting spirit on court.</t>
   </si>
   <si>
     <t xml:space="preserve">Peter Lucassen</t>
@@ -273,7 +273,7 @@
     <t xml:space="preserve">Big serve, Mr. Nice Guy, powerful serve, aggressive, composed</t>
   </si>
   <si>
-    <t xml:space="preserve">“Raonic's game is built around his powerful serve, which is one of the best in the men's game. He also has powerful groundstrokes and seeks to play aggressively, often looking to finish points at the net. He's worked to improve his mobility and baseline game throughout his career."</t>
+    <t xml:space="preserve">Raonic's game is built around his powerful serve, which is one of the best in the men's game. He also has powerful groundstrokes and seeks to play aggressively, often looking to finish points at the net. He's worked to improve his mobility and baseline game throughout his career.</t>
   </si>
   <si>
     <t xml:space="preserve">Mario Tudor</t>
@@ -291,7 +291,7 @@
     <t xml:space="preserve">Outspoken, interactive, local hero, powerful serve</t>
   </si>
   <si>
-    <t xml:space="preserve">“Known for his powerful serve and aggressive baseline play. "</t>
+    <t xml:space="preserve">Known for his powerful serve and aggressive baseline play. </t>
   </si>
   <si>
     <t xml:space="preserve">Kristof Vliegen</t>
@@ -309,7 +309,7 @@
     <t xml:space="preserve">consistent, fighting spirit, groundstroke</t>
   </si>
   <si>
-    <t xml:space="preserve">“Kecmanovic is a steady baseliner with solid groundstrokes from both wings. He has a well-rounded game, with no significant weaknesses, and he's known for his fighting spirit and ability to maintain a high level of play under pressure."</t>
+    <t xml:space="preserve">Kecmanovic is a steady baseliner with solid groundstrokes from both wings. He has a well-rounded game, with no significant weaknesses, and he's known for his fighting spirit and ability to maintain a high level of play under pressure.</t>
   </si>
   <si>
     <t xml:space="preserve">Wayne Black, Ivan Cinkus</t>
@@ -324,7 +324,7 @@
     <t xml:space="preserve">Emotional, funny, interactive, patient, clay-court specialist</t>
   </si>
   <si>
-    <t xml:space="preserve">“A Spanish tennis player, Miralles is known for his clay-court skills, which are typical of many Spanish players. His game is characterised by heavy topspin from the baseline, particularly on the forehand side, and a patient approach, often waiting for his opponent to make errors rather than going for outright winners."</t>
+    <t xml:space="preserve">A Spanish tennis player, Miralles is known for his clay-court skills, which are typical of many Spanish players. His game is characterised by heavy topspin from the baseline, particularly on the forehand side, and a patient approach, often waiting for his opponent to make errors rather than going for outright winners.</t>
   </si>
   <si>
     <t xml:space="preserve">Samuel Ribeiro</t>
@@ -342,7 +342,7 @@
     <t xml:space="preserve">Focused, shy, quiet, energetic</t>
   </si>
   <si>
-    <t xml:space="preserve">“A player with an aggressive playing style, Cressy is notable for his serve-and-volley tactics, a relatively rare strategy in modern tennis. He possesses a powerful serve and isn't afraid to approach the net, looking to finish points quickly."</t>
+    <t xml:space="preserve">A player with an aggressive playing style, Cressy is notable for his serve-and-volley tactics, a relatively rare strategy in modern tennis. He possesses a powerful serve and isn't afraid to approach the net, looking to finish points quickly.</t>
   </si>
   <si>
     <t xml:space="preserve">Alexandre Sidorenko, Juanjo Climent, Andrew Mawire </t>
@@ -360,7 +360,7 @@
     <t xml:space="preserve">Focused, cool, consistent</t>
   </si>
   <si>
-    <t xml:space="preserve">“ Ruusuvuori has a solid baseline game, powerful from both wings, with a particular strength in his backhand. He's also known for his fighting spirit and mental toughness on the court. Off the court, he has diverse interests from music to hockey."</t>
+    <t xml:space="preserve">Ruusuvuori has a solid baseline game, powerful from both wings, with a particular strength in his backhand. He's also known for his fighting spirit and mental toughness on the court. Off the court, he has diverse interests from music to hockey.</t>
   </si>
   <si>
     <t xml:space="preserve">Federico Ricci</t>
@@ -384,7 +384,7 @@
     <t xml:space="preserve">Creative, focused, quiet, precise, groundstroke, unorthodox</t>
   </si>
   <si>
-    <t xml:space="preserve">“Mannarino is known for his unorthodox playing style. He has a flat groundstroke and an excellent sense of timing, often disrupting opponents with unpredictable shot selection. He is also known for his excellent footwork and defensive skills."</t>
+    <t xml:space="preserve">Mannarino is known for his unorthodox playing style. He has a flat groundstroke and an excellent sense of timing, often disrupting opponents with unpredictable shot selection. He is also known for his excellent footwork and defensive skills.</t>
   </si>
   <si>
     <t xml:space="preserve">Erwann Tortuyaux</t>
@@ -399,7 +399,7 @@
     <t xml:space="preserve">Perfectionist, well-schooled, composed</t>
   </si>
   <si>
-    <t xml:space="preserve">“Nakashima has a powerful baseline game, especially his backhand, and is known for his tactical intelligence and composure on court. His serve is also a significant weapon, allowing him to control many points from the onset."</t>
+    <t xml:space="preserve">Nakashima has a powerful baseline game, especially his backhand, and is known for his tactical intelligence and composure on court. His serve is also a significant weapon, allowing him to control many points from the onset.</t>
   </si>
   <si>
     <t xml:space="preserve">Edwardo Infantino</t>
@@ -417,7 +417,7 @@
     <t xml:space="preserve">Showman, outspoken, interactive, unpredictable, entertaining</t>
   </si>
   <si>
-    <t xml:space="preserve">“Bublik is known for his unpredictable and often flashy style of play. He has a powerful serve and isn't afraid to use underarm serves to catch his opponents off guard. He also frequently employs drop shots and has a strong net game."</t>
+    <t xml:space="preserve">Bublik is known for his unpredictable and often flashy style of play. He has a powerful serve and isn't afraid to use underarm serves to catch his opponents off guard. He also frequently employs drop shots and has a strong net game.</t>
   </si>
   <si>
     <t xml:space="preserve">Artem Suprunov</t>
@@ -432,7 +432,7 @@
     <t xml:space="preserve">aggressive, focused, powerful serve, powerful forehand, quiet</t>
   </si>
   <si>
-    <t xml:space="preserve">“A left-handed player, Humbert is known for his aggressive all-court game. He has a strong serve and a potent one-handed backhand, and he likes to take control of points early. He's also known for his ability to vary the pace and spin of his shots, often keeping opponents off balance."</t>
+    <t xml:space="preserve">A left-handed player, Humbert is known for his aggressive all-court game. He has a strong serve and a potent one-handed backhand, and he likes to take control of points early. He's also known for his ability to vary the pace and spin of his shots, often keeping opponents off balance.</t>
   </si>
   <si>
     <t xml:space="preserve">Jeremy Chardy</t>
@@ -450,7 +450,7 @@
     <t xml:space="preserve">Big serve, local hero, speedy, agile, fighting spirit</t>
   </si>
   <si>
-    <t xml:space="preserve">“Ymer is a steady baseline player with a solid two-handed backhand. He's known for his speed and athleticism on the court, often engaging opponents in long rallies and outlasting them with his physicality and endurance."</t>
+    <t xml:space="preserve">Ymer is a steady baseline player with a solid two-handed backhand. He's known for his speed and athleticism on the court, often engaging opponents in long rallies and outlasting them with his physicality and endurance.</t>
   </si>
   <si>
     <t xml:space="preserve">Daniel Berta</t>
@@ -468,7 +468,7 @@
     <t xml:space="preserve">powerful serve, powerful groundstroke, aggressive</t>
   </si>
   <si>
-    <t xml:space="preserve">“van Rijthoven has a game that is characterized by a strong serve and an aggressive baseline play. He prefers hard courts and isn't afraid to approach the net, often looking to finish points quickly."</t>
+    <t xml:space="preserve">van Rijthoven has a game that is characterized by a strong serve and an aggressive baseline play. He prefers hard courts and isn't afraid to approach the net, often looking to finish points quickly.</t>
   </si>
   <si>
     <t xml:space="preserve">Igor Sijsling</t>
@@ -486,7 +486,10 @@
     <t xml:space="preserve">Olympian, groundstroke, tactical, defensive, serve, footwork</t>
   </si>
   <si>
-    <t xml:space="preserve">“Bencic possesses a versatile game marked by excellent court coverage and an ability to change direction of the ball with ease. Her smart tactical sense allows her to construct points effectively, often outmaneuvering her opponents with precise shot placement."</t>
+    <t xml:space="preserve">“Bencic possesses a versatile game marked by excellent court coverage and an ability to change direction of the ball with ease. Her smart tactical sense allows her to construct points effectively, often outmaneuvering her opponents with precise shot placement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dmitry Tursunov</t>
   </si>
   <si>
     <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Bencic_Hero-Smile.webp</t>
@@ -501,7 +504,7 @@
     <t xml:space="preserve">serve, forehand, net game, backhand</t>
   </si>
   <si>
-    <t xml:space="preserve">“Kudermetova has a strong baseline game, characterized by powerful groundstrokes. She has an aggressive style of play, often looking to dictate points with her strong serve and forehand."</t>
+    <t xml:space="preserve">“Kudermetova has a strong baseline game, characterized by powerful groundstrokes. She has an aggressive style of play, often looking to dictate points with her strong serve and forehand.</t>
   </si>
   <si>
     <t xml:space="preserve">Sergey Demekhine, Vladimir Platenik</t>
@@ -516,7 +519,10 @@
     <t xml:space="preserve">Long games, groundstrokes, aggressive, serve, consistent, mental toughness</t>
   </si>
   <si>
-    <t xml:space="preserve">“Samsonova is known for her aggressive game. She has powerful groundstrokes from both wings and a strong serve, which allows her to dictate play and keep opponents on the back foot."</t>
+    <t xml:space="preserve">“Samsonova is known for her aggressive game. She has powerful groundstrokes from both wings and a strong serve, which allows her to dictate play and keep opponents on the back foot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alessandro Dumitrache</t>
   </si>
   <si>
     <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Samsonova_Crop.webp</t>
@@ -528,7 +534,7 @@
     <t xml:space="preserve">Outspoken, fighter, showman, Consistent, movement, groundstrokes, serve, competitive</t>
   </si>
   <si>
-    <t xml:space="preserve">“A former world No. 1, Azarenka's game is characterized by her powerful baseline play and strong return of serve, often taking the ball early and redirecting with pace. She's also noted for her mental toughness and competitive spirit on court."</t>
+    <t xml:space="preserve">“A former world No. 1, Azarenka's game is characterized by her powerful baseline play and strong return of serve, often taking the ball early and redirecting with pace. She's also noted for her mental toughness and competitive spirit on court.</t>
   </si>
   <si>
     <t xml:space="preserve">Maxime Tchoutakian</t>
@@ -546,7 +552,7 @@
     <t xml:space="preserve">Talented, Versatile, strong groundstrokes, powerful serve, aggressive, net play</t>
   </si>
   <si>
-    <t xml:space="preserve">“Zheng is a young player known for her aggressive game style, with a powerful serve and strong groundstrokes. She often looks to dictate the play and isn't afraid to go for winners."</t>
+    <t xml:space="preserve">“Zheng is a young player known for her aggressive game style, with a powerful serve and strong groundstrokes. She often looks to dictate the play and isn't afraid to go for winners.</t>
   </si>
   <si>
     <t xml:space="preserve">Pedro Riba Madrid</t>
@@ -561,7 +567,7 @@
     <t xml:space="preserve">Quiet, serve, aggressive, forehand, consistent, mental toughness</t>
   </si>
   <si>
-    <t xml:space="preserve">“Alexandrova is known for her aggressive baseline game. She possesses a powerful serve and forehand, often looking to finish points quickly rather than engage in extended rallies."</t>
+    <t xml:space="preserve">“Alexandrova is known for her aggressive baseline game. She possesses a powerful serve and forehand, often looking to finish points quickly rather than engage in extended rallies.</t>
   </si>
   <si>
     <t xml:space="preserve">Evgeny Alexandrova</t>
@@ -579,7 +585,7 @@
     <t xml:space="preserve">Lovely, respectful, interactive, Consistent, footwork, groundstrokes, serve, defensive</t>
   </si>
   <si>
-    <t xml:space="preserve">“Mertens has a well-rounded game, marked by solid groundstrokes, good court coverage and tactical intelligence. Her versatile game allows her to adapt to different playing styles and court surfaces."</t>
+    <t xml:space="preserve">“Mertens has a well-rounded game, marked by solid groundstrokes, good court coverage and tactical intelligence. Her versatile game allows her to adapt to different playing styles and court surfaces.</t>
   </si>
   <si>
     <t xml:space="preserve">Alexander Kneepkens</t>
@@ -594,7 +600,7 @@
     <t xml:space="preserve">Well-trained, groundstrokes, tactical, serve, net play, defensive</t>
   </si>
   <si>
-    <t xml:space="preserve">“Martic is a strategic player known for her variety, often mixing up pace and spin to disrupt her opponent's rhythm. She has a strong serve and is particularly effective at the net, with good volleying skills."</t>
+    <t xml:space="preserve">“Martic is a strategic player known for her variety, often mixing up pace and spin to disrupt her opponent's rhythm. She has a strong serve and is particularly effective at the net, with good volleying skills.</t>
   </si>
   <si>
     <t xml:space="preserve">Michael Geserer</t>
@@ -609,7 +615,7 @@
     <t xml:space="preserve">Talented, entertaining, fighter, Versatile, groundstrokes, aggressive, serve, competitive</t>
   </si>
   <si>
-    <t xml:space="preserve">“Andreescu's game is characterized by its variety and power. She has strong groundstrokes, a potent serve, and isn't afraid to come forward and finish points at the net. She also uses a variety of spins and paces to disrupt her opponents."</t>
+    <t xml:space="preserve">“Andreescu's game is characterized by its variety and power. She has strong groundstrokes, a potent serve, and isn't afraid to come forward and finish points at the net. She also uses a variety of spins and paces to disrupt her opponents.</t>
   </si>
   <si>
     <t xml:space="preserve">Christphe Lambert</t>
@@ -624,7 +630,7 @@
     <t xml:space="preserve">serve, groundstrokes, aggressive, net play, mental toughness</t>
   </si>
   <si>
-    <t xml:space="preserve">“Rogers is known for her powerful serve and aggressive baseline play. She has a strong forehand and isn't afraid to attack and dictate the play, often seeking to finish points quickly."</t>
+    <t xml:space="preserve">“Rogers is known for her powerful serve and aggressive baseline play. She has a strong forehand and isn't afraid to attack and dictate the play, often seeking to finish points quickly.</t>
   </si>
   <si>
     <t xml:space="preserve">Piotr Sierzputowski</t>
@@ -642,7 +648,7 @@
     <t xml:space="preserve">Positive, runs a lot, Consistent, groundstrokes, movement, defensive, serve</t>
   </si>
   <si>
-    <t xml:space="preserve">“Bouzkova is known for her consistent baseline game and good court coverage. She has solid groundstrokes and a good defensive game, often forcing opponents into errors."</t>
+    <t xml:space="preserve">“Bouzkova is known for her consistent baseline game and good court coverage. She has solid groundstrokes and a good defensive game, often forcing opponents into errors.</t>
   </si>
   <si>
     <t xml:space="preserve">Cristian Requeni, Milan Bouzek</t>
@@ -660,7 +666,7 @@
     <t xml:space="preserve">Versatile, groundstrokes, serve, consistency, tactical</t>
   </si>
   <si>
-    <t xml:space="preserve">“Sasnovich is a consistent player with solid groundstrokes from both wings. She often plays a patient game from the baseline, waiting for her opponents to make errors."</t>
+    <t xml:space="preserve">“Sasnovich is a consistent player with solid groundstrokes from both wings. She often plays a patient game from the baseline, waiting for her opponents to make errors.</t>
   </si>
   <si>
     <t xml:space="preserve">Dzmitry Klimenko</t>
@@ -675,7 +681,7 @@
     <t xml:space="preserve">serve, aggressive, groundstrokes, consistent, footwork</t>
   </si>
   <si>
-    <t xml:space="preserve">“Gracheva's game is characterized by her solid baseline play and consistent groundstrokes. She has a patient approach to her game, often engaging in long rallies and waiting for her opponent to make errors."</t>
+    <t xml:space="preserve">“Gracheva's game is characterized by her solid baseline play and consistent groundstrokes. She has a patient approach to her game, often engaging in long rallies and waiting for her opponent to make errors.</t>
   </si>
   <si>
     <t xml:space="preserve">Xavier Pujo</t>
@@ -690,7 +696,7 @@
     <t xml:space="preserve">Versatile, serve, groundstrokes, aggressive, net play</t>
   </si>
   <si>
-    <t xml:space="preserve">“Muchova has a versatile game, with a good mix of power and finesse. She often employs a variety of shots, including slices and drop shots, to disrupt her opponent's rhythm."</t>
+    <t xml:space="preserve">“Muchova has a versatile game, with a good mix of power and finesse. She often employs a variety of shots, including slices and drop shots, to disrupt her opponent's rhythm.</t>
   </si>
   <si>
     <t xml:space="preserve">David Kotyza</t>
@@ -732,7 +738,7 @@
     <t xml:space="preserve">Consistent, tactical, changes pace, court awareness</t>
   </si>
   <si>
-    <t xml:space="preserve">“Evgeniya Rodina is a seasoned player with a well-rounded game. Known for her consistency and tactical intelligence, she can change up the pace and spin of her shots to disrupt her opponent's rhythm. While not the most powerful player on tour, Rodina uses her court awareness and shot selection effectively to construct points."</t>
+    <t xml:space="preserve">“Evgeniya Rodina is a seasoned player with a well-rounded game. Known for her consistency and tactical intelligence, she can change up the pace and spin of her shots to disrupt her opponent's rhythm. While not the most powerful player on tour, Rodina uses her court awareness and shot selection effectively to construct points.</t>
   </si>
   <si>
     <t xml:space="preserve">Oxana Mishikova</t>
@@ -747,7 +753,7 @@
     <t xml:space="preserve">Aggressive, positive, powerful groundstrokes, strong serve, net play, tough competitor</t>
   </si>
   <si>
-    <t xml:space="preserve">“Alison Riske-Amritraj is known for her aggressive baseline play and powerful groundstrokes. Her strengths include a strong serve and a particularly effective backhand. She also has a knack for coming to the net, showcasing her versatile skill set. Over the years, Riske-Amritraj has developed a reputation for being a tough competitor, often playing her best tennis in tight situations."</t>
+    <t xml:space="preserve">“Alison Riske-Amritraj is known for her aggressive baseline play and powerful groundstrokes. Her strengths include a strong serve and a particularly effective backhand. She also has a knack for coming to the net, showcasing her versatile skill set. Over the years, Riske-Amritraj has developed a reputation for being a tough competitor, often playing her best tennis in tight situations.</t>
   </si>
   <si>
     <t xml:space="preserve">Thomas Gutteridge</t>
@@ -762,7 +768,7 @@
     <t xml:space="preserve">Left-handed, powerful serve, topspin forehand, aggressive, high-risk</t>
   </si>
   <si>
-    <t xml:space="preserve">“Ysaline Bonaventure is a left-handed player known for her powerful serve and heavy topspin forehand. Her game is characterized by aggressive shot-making and the ability to generate pace from both wings. While she can be erratic at times, her high-risk style of play can be very effective when she's in form."</t>
+    <t xml:space="preserve">“Ysaline Bonaventure is a left-handed player known for her powerful serve and heavy topspin forehand. Her game is characterized by aggressive shot-making and the ability to generate pace from both wings. While she can be erratic at times, her high-risk style of play can be very effective when she's in form.</t>
   </si>
   <si>
     <t xml:space="preserve">Hugo Guerriero</t>
@@ -777,7 +783,7 @@
     <t xml:space="preserve">Baseline player, consistent, strong groundstrokes, defensive, counterpunching, fighting spirit</t>
   </si>
   <si>
-    <t xml:space="preserve">“Rebecca Peterson is a solid baseline player with a consistent game. She uses her strong groundstrokes to construct points and can change direction of the ball effectively. Peterson also has a good defensive game, often turning defense into offense with her counterpunching ability. She's known for her fighting spirit on the court, often grinding out tough matches."</t>
+    <t xml:space="preserve">“Rebecca Peterson is a solid baseline player with a consistent game. She uses her strong groundstrokes to construct points and can change direction of the ball effectively. Peterson also has a good defensive game, often turning defense into offense with her counterpunching ability. She's known for her fighting spirit on the court, often grinding out tough matches.</t>
   </si>
   <si>
     <t xml:space="preserve">Mart Peterson</t>
@@ -795,7 +801,7 @@
     <t xml:space="preserve">groundstrokes, aggressive</t>
   </si>
   <si>
-    <t xml:space="preserve">“Anna-Lena Friedsam is an aggressive baseliner who relies on her powerful groundstrokes to dictate play. She looks to take control of the rallies by hitting aggressive shots and going for winners. At the same time, she has the ability to defend and counter-punch effectively, adjusting her game according to the situation."</t>
+    <t xml:space="preserve">“Anna-Lena Friedsam is an aggressive baseliner who relies on her powerful groundstrokes to dictate play. She looks to take control of the rallies by hitting aggressive shots and going for winners. At the same time, she has the ability to defend and counter-punch effectively, adjusting her game according to the situation.</t>
   </si>
   <si>
     <t xml:space="preserve">Patrice Hopfe</t>
@@ -813,10 +819,13 @@
     <t xml:space="preserve">Consistent, excellent movement, defensive skills, solid groundstrokes, mental toughness, competitive spirit</t>
   </si>
   <si>
-    <t xml:space="preserve">“Elina Svitolina is one of the most consistent players on the WTA Tour, known for her excellent movement, strong defensive skills, and the ability to turn defense into offense. Her game is based around her solid groundstrokes and her ability to move her opponents around the court. Svitolina is also known for her mental toughness and strong competitive spirit, often elevating her game in important moments."</t>
+    <t xml:space="preserve">“Elina Svitolina is one of the most consistent players on the WTA Tour, known for her excellent movement, strong defensive skills, and the ability to turn defense into offense. Her game is based around her solid groundstrokes and her ability to move her opponents around the court. Svitolina is also known for her mental toughness and strong competitive spirit, often elevating her game in important moments.</t>
   </si>
   <si>
     <t xml:space="preserve">Raemon Sluiter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://libema-open.nl/wp-content/uploads/2023/05/Svitolina_Hero-Smile.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Styles</t>
@@ -909,7 +918,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -938,6 +947,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -947,7 +964,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -961,12 +978,38 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF006600"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1003,7 +1046,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1032,12 +1075,12 @@
   </sheetPr>
   <dimension ref="A1:Y1021"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="K20" activeCellId="0" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1054,127 +1097,127 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>198</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="L2" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <v>2014</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P2" s="1" t="n">
         <f aca="false">2023-O2</f>
         <v>9</v>
       </c>
@@ -1190,10 +1233,10 @@
         <f aca="false">IF(B2=M2,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="U2" s="0" t="str">
+      <c r="U2" s="1" t="str">
         <f aca="false">IF(B2=M2,"All time high","")</f>
         <v/>
       </c>
@@ -1201,61 +1244,64 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="W2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="Y2" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>193</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="L3" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <v>2017</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="P3" s="1" t="n">
         <f aca="false">2023-O3</f>
         <v>6</v>
       </c>
@@ -1271,10 +1317,10 @@
         <f aca="false">IF(B3=M3,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="T3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U3" s="0" t="str">
+      <c r="U3" s="1" t="str">
         <f aca="false">IF(B3=M3,"All time high","")</f>
         <v/>
       </c>
@@ -1282,61 +1328,64 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="W3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="Y3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="1" t="s">
         <v>46</v>
       </c>
       <c r="L4" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="O4" s="1" t="n">
         <v>2013</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="P4" s="1" t="n">
         <f aca="false">2023-O4</f>
         <v>10</v>
       </c>
@@ -1352,10 +1401,10 @@
         <f aca="false">IF(B4=M4,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="T4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="U4" s="0" t="str">
+      <c r="U4" s="1" t="str">
         <f aca="false">IF(B4=M4,"All time high","")</f>
         <v/>
       </c>
@@ -1363,61 +1412,64 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="X4" s="0" t="s">
+      <c r="W4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Y4" s="0" t="s">
+      <c r="Y4" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>183</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="K5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="L5" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="M5" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="O5" s="0" t="n">
+      <c r="O5" s="1" t="n">
         <v>2015</v>
       </c>
-      <c r="P5" s="0" t="n">
+      <c r="P5" s="1" t="n">
         <f aca="false">2023-O5</f>
         <v>8</v>
       </c>
@@ -1433,10 +1485,10 @@
         <f aca="false">IF(B5=M5,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T5" s="0" t="s">
+      <c r="T5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="U5" s="0" t="str">
+      <c r="U5" s="1" t="str">
         <f aca="false">IF(B5=M5,"All time high","")</f>
         <v/>
       </c>
@@ -1444,30 +1496,33 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="X5" s="0" t="s">
+      <c r="W5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Y5" s="0" t="s">
+      <c r="Y5" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -1479,26 +1534,26 @@
       <c r="I6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="K6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="L6" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6" s="1" t="n">
         <v>2017</v>
       </c>
-      <c r="O6" s="0" t="n">
+      <c r="O6" s="1" t="n">
         <v>2009</v>
       </c>
-      <c r="P6" s="0" t="n">
+      <c r="P6" s="1" t="n">
         <f aca="false">2023-O6</f>
         <v>14</v>
       </c>
@@ -1514,10 +1569,10 @@
         <f aca="false">IF(B6=M6,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T6" s="0" t="s">
+      <c r="T6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U6" s="0" t="str">
+      <c r="U6" s="1" t="str">
         <f aca="false">IF(B6=M6,"All time high","")</f>
         <v/>
       </c>
@@ -1525,30 +1580,33 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W6" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X6" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="Y6" s="0" t="s">
+      <c r="Y6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>198</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1560,26 +1618,26 @@
       <c r="I7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K7" s="1" t="s">
         <v>64</v>
       </c>
       <c r="L7" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="O7" s="0" t="n">
+      <c r="O7" s="1" t="n">
         <v>2005</v>
       </c>
-      <c r="P7" s="0" t="n">
+      <c r="P7" s="1" t="n">
         <f aca="false">2023-O7</f>
         <v>18</v>
       </c>
@@ -1595,10 +1653,10 @@
         <f aca="false">IF(B7=M7,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T7" s="0" t="s">
+      <c r="T7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="U7" s="0" t="str">
+      <c r="U7" s="1" t="str">
         <f aca="false">IF(B7=M7,"All time high","")</f>
         <v/>
       </c>
@@ -1606,30 +1664,33 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W7" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="Y7" s="0" t="s">
+      <c r="Y7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>193</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1641,22 +1702,26 @@
       <c r="I8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="K8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="L8" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="N8" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="O8" s="1" t="n">
         <v>2005</v>
       </c>
-      <c r="P8" s="0" t="n">
+      <c r="P8" s="1" t="n">
         <f aca="false">2023-O8</f>
         <v>18</v>
       </c>
@@ -1672,10 +1737,10 @@
         <f aca="false">IF(B8=M8,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T8" s="0" t="s">
+      <c r="T8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="U8" s="0" t="str">
+      <c r="U8" s="1" t="str">
         <f aca="false">IF(B8=M8,"All time high","")</f>
         <v/>
       </c>
@@ -1683,36 +1748,36 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W8" s="0" t="n">
+      <c r="W8" s="1" t="n">
         <v>2014</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="Y8" s="0" t="s">
+      <c r="Y8" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>191</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -1721,26 +1786,26 @@
       <c r="I9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="K9" s="1" t="s">
         <v>76</v>
       </c>
       <c r="L9" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M9" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N9" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="O9" s="1" t="n">
         <v>2016</v>
       </c>
-      <c r="P9" s="0" t="n">
+      <c r="P9" s="1" t="n">
         <f aca="false">2023-O9</f>
         <v>7</v>
       </c>
@@ -1756,10 +1821,10 @@
         <f aca="false">IF(B9=M9,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T9" s="0" t="s">
+      <c r="T9" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="U9" s="0" t="str">
+      <c r="U9" s="1" t="str">
         <f aca="false">IF(B9=M9,"All time high","")</f>
         <v/>
       </c>
@@ -1767,30 +1832,33 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W9" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X9" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="Y9" s="0" t="s">
+      <c r="Y9" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>196</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1802,22 +1870,26 @@
       <c r="I10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="J10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="0" t="s">
+      <c r="K10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="L10" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="N10" s="0" t="n">
+      <c r="N10" s="1" t="n">
         <v>2016</v>
       </c>
-      <c r="O10" s="0" t="n">
+      <c r="O10" s="1" t="n">
         <v>2008</v>
       </c>
-      <c r="P10" s="0" t="n">
+      <c r="P10" s="1" t="n">
         <f aca="false">2023-O10</f>
         <v>15</v>
       </c>
@@ -1833,7 +1905,7 @@
         <f aca="false">IF(B10=M10,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T10" s="0" t="s">
+      <c r="T10" s="1" t="s">
         <v>83</v>
       </c>
       <c r="U10" s="2" t="s">
@@ -1843,33 +1915,36 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W10" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X10" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="Y10" s="0" t="s">
+      <c r="Y10" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="1" t="s">
         <v>38</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -1878,26 +1953,26 @@
       <c r="I11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="J11" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K11" s="0" t="s">
+      <c r="K11" s="1" t="s">
         <v>88</v>
       </c>
       <c r="L11" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="O11" s="0" t="n">
+      <c r="O11" s="1" t="n">
         <v>2015</v>
       </c>
-      <c r="P11" s="0" t="n">
+      <c r="P11" s="1" t="n">
         <f aca="false">2023-O11</f>
         <v>8</v>
       </c>
@@ -1913,10 +1988,10 @@
         <f aca="false">IF(B11=M11,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T11" s="0" t="s">
+      <c r="T11" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="U11" s="0" t="str">
+      <c r="U11" s="1" t="str">
         <f aca="false">IF(B11=M11,"All time high","")</f>
         <v/>
       </c>
@@ -1924,30 +1999,33 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W11" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X11" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="Y11" s="0" t="s">
+      <c r="Y11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>183</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="1" t="s">
         <v>92</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1959,26 +2037,26 @@
       <c r="I12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="J12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K12" s="0" t="s">
+      <c r="K12" s="1" t="s">
         <v>94</v>
       </c>
       <c r="L12" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M12" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N12" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="O12" s="0" t="n">
+      <c r="O12" s="1" t="n">
         <v>2017</v>
       </c>
-      <c r="P12" s="0" t="n">
+      <c r="P12" s="1" t="n">
         <f aca="false">2023-O12</f>
         <v>6</v>
       </c>
@@ -1994,10 +2072,10 @@
         <f aca="false">IF(B12=M12,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T12" s="0" t="s">
+      <c r="T12" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="U12" s="0" t="str">
+      <c r="U12" s="1" t="str">
         <f aca="false">IF(B12=M12,"All time high","")</f>
         <v/>
       </c>
@@ -2005,33 +2083,36 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W12" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X12" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="Y12" s="0" t="s">
+      <c r="Y12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>183</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" s="1" t="s">
         <v>38</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -2040,26 +2121,26 @@
       <c r="I13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="J13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K13" s="0" t="s">
+      <c r="K13" s="1" t="s">
         <v>99</v>
       </c>
       <c r="L13" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M13" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N13" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="O13" s="0" t="n">
+      <c r="O13" s="1" t="n">
         <v>2015</v>
       </c>
-      <c r="P13" s="0" t="n">
+      <c r="P13" s="1" t="n">
         <f aca="false">2023-O13</f>
         <v>8</v>
       </c>
@@ -2075,10 +2156,10 @@
         <f aca="false">IF(B13=M13,TRUE(),FALSE())</f>
         <v>1</v>
       </c>
-      <c r="T13" s="0" t="s">
+      <c r="T13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="U13" s="0" t="str">
+      <c r="U13" s="1" t="str">
         <f aca="false">IF(B13=M13,"All time high","")</f>
         <v>All time high</v>
       </c>
@@ -2086,33 +2167,36 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W13" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X13" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="Y13" s="0" t="s">
+      <c r="Y13" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>201</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" s="1" t="s">
         <v>62</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -2121,26 +2205,26 @@
       <c r="I14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J14" s="0" t="s">
+      <c r="J14" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K14" s="0" t="s">
+      <c r="K14" s="1" t="s">
         <v>105</v>
       </c>
       <c r="L14" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="M14" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="N14" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="O14" s="0" t="n">
+      <c r="O14" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="P14" s="0" t="n">
+      <c r="P14" s="1" t="n">
         <f aca="false">2023-O14</f>
         <v>4</v>
       </c>
@@ -2159,7 +2243,7 @@
       <c r="T14" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="U14" s="0" t="str">
+      <c r="U14" s="1" t="str">
         <f aca="false">IF(B14=M14,"All time high","")</f>
         <v/>
       </c>
@@ -2167,33 +2251,36 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W14" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X14" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="Y14" s="0" t="s">
+      <c r="Y14" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="1" t="s">
         <v>38</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -2202,7 +2289,7 @@
       <c r="I15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="J15" s="1" t="s">
         <v>110</v>
       </c>
       <c r="K15" s="6" t="s">
@@ -2212,16 +2299,16 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="N15" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="O15" s="0" t="n">
+      <c r="O15" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="P15" s="0" t="n">
+      <c r="P15" s="1" t="n">
         <f aca="false">2023-O15</f>
         <v>5</v>
       </c>
@@ -2237,10 +2324,10 @@
         <f aca="false">IF(B15=M15,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T15" s="0" t="s">
+      <c r="T15" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="U15" s="0" t="str">
+      <c r="U15" s="1" t="str">
         <f aca="false">IF(B15=M15,"All time high","")</f>
         <v/>
       </c>
@@ -2248,61 +2335,64 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W15" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X15" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="Y15" s="0" t="s">
+      <c r="Y15" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>37</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="0" t="s">
+      <c r="J16" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="K16" s="0" t="s">
+      <c r="K16" s="1" t="s">
         <v>119</v>
       </c>
       <c r="L16" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="M16" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="N16" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="O16" s="0" t="n">
+      <c r="O16" s="1" t="n">
         <v>2004</v>
       </c>
-      <c r="P16" s="0" t="n">
+      <c r="P16" s="1" t="n">
         <f aca="false">2023-O16</f>
         <v>19</v>
       </c>
@@ -2318,10 +2408,10 @@
         <f aca="false">IF(B16=M16,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T16" s="0" t="s">
+      <c r="T16" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="U16" s="0" t="str">
+      <c r="U16" s="1" t="str">
         <f aca="false">IF(B16=M16,"All time high","")</f>
         <v/>
       </c>
@@ -2329,64 +2419,64 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W16" s="0" t="n">
+      <c r="W16" s="1" t="n">
         <v>2019</v>
       </c>
       <c r="X16" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="Y16" s="0" t="s">
+      <c r="Y16" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>52</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G17" s="0" t="s">
+      <c r="G17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="H17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="I17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="0" t="s">
+      <c r="J17" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="K17" s="0" t="s">
+      <c r="K17" s="1" t="s">
         <v>124</v>
       </c>
       <c r="L17" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="M17" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="N17" s="0" t="n">
+      <c r="N17" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="O17" s="0" t="n">
+      <c r="O17" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="P17" s="0" t="n">
+      <c r="P17" s="1" t="n">
         <f aca="false">2023-O17</f>
         <v>4</v>
       </c>
@@ -2402,10 +2492,10 @@
         <f aca="false">IF(B17=M17,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T17" s="0" t="s">
+      <c r="T17" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="U17" s="0" t="str">
+      <c r="U17" s="1" t="str">
         <f aca="false">IF(B17=M17,"All time high","")</f>
         <v/>
       </c>
@@ -2413,61 +2503,64 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W17" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X17" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="Y17" s="0" t="s">
+      <c r="Y17" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>48</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>196</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="G18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="H18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="0" t="s">
+      <c r="I18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J18" s="0" t="s">
+      <c r="J18" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K18" s="0" t="s">
+      <c r="K18" s="1" t="s">
         <v>130</v>
       </c>
       <c r="L18" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M18" s="0" t="n">
+      <c r="M18" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="N18" s="0" t="n">
+      <c r="N18" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="O18" s="0" t="n">
+      <c r="O18" s="1" t="n">
         <v>2016</v>
       </c>
-      <c r="P18" s="0" t="n">
+      <c r="P18" s="1" t="n">
         <f aca="false">2023-O18</f>
         <v>7</v>
       </c>
@@ -2483,10 +2576,10 @@
         <f aca="false">IF(B18=M18,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T18" s="0" t="s">
+      <c r="T18" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="U18" s="0" t="str">
+      <c r="U18" s="1" t="str">
         <f aca="false">IF(B18=M18,"All time high","")</f>
         <v/>
       </c>
@@ -2494,61 +2587,64 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W18" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X18" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="Y18" s="0" t="s">
+      <c r="Y18" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="H19" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="I19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="0" t="s">
+      <c r="J19" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="K19" s="0" t="s">
+      <c r="K19" s="1" t="s">
         <v>135</v>
       </c>
       <c r="L19" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M19" s="0" t="n">
+      <c r="M19" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="N19" s="0" t="n">
+      <c r="N19" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="O19" s="0" t="n">
+      <c r="O19" s="1" t="n">
         <v>2016</v>
       </c>
-      <c r="P19" s="0" t="n">
+      <c r="P19" s="1" t="n">
         <f aca="false">2023-O19</f>
         <v>7</v>
       </c>
@@ -2564,10 +2660,10 @@
         <f aca="false">IF(B19=M19,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T19" s="0" t="s">
+      <c r="T19" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="U19" s="0" t="str">
+      <c r="U19" s="1" t="str">
         <f aca="false">IF(B19=M19,"All time high","")</f>
         <v/>
       </c>
@@ -2575,61 +2671,64 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W19" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X19" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="Y19" s="0" t="s">
+      <c r="Y19" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>53</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>183</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="G20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="0" t="s">
+      <c r="H20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="I20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J20" s="0" t="s">
+      <c r="J20" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K20" s="0" t="s">
+      <c r="K20" s="1" t="s">
         <v>141</v>
       </c>
       <c r="L20" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="M20" s="0" t="n">
+      <c r="M20" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="N20" s="0" t="n">
+      <c r="N20" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="O20" s="0" t="n">
+      <c r="O20" s="1" t="n">
         <v>2015</v>
       </c>
-      <c r="P20" s="0" t="n">
+      <c r="P20" s="1" t="n">
         <f aca="false">2023-O20</f>
         <v>8</v>
       </c>
@@ -2645,10 +2744,10 @@
         <f aca="false">IF(B20=M20,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T20" s="0" t="s">
+      <c r="T20" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="U20" s="0" t="str">
+      <c r="U20" s="1" t="str">
         <f aca="false">IF(B20=M20,"All time high","")</f>
         <v/>
       </c>
@@ -2656,61 +2755,64 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="W20" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X20" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="Y20" s="0" t="s">
+      <c r="Y20" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>157</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="G21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="H21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J21" s="0" t="s">
+      <c r="J21" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="K21" s="0" t="s">
+      <c r="K21" s="1" t="s">
         <v>147</v>
       </c>
       <c r="L21" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M21" s="0" t="n">
+      <c r="M21" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="N21" s="0" t="n">
+      <c r="N21" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="O21" s="0" t="n">
+      <c r="O21" s="1" t="n">
         <v>2015</v>
       </c>
-      <c r="P21" s="0" t="n">
+      <c r="P21" s="1" t="n">
         <f aca="false">2023-O21</f>
         <v>8</v>
       </c>
@@ -2726,10 +2828,10 @@
         <f aca="false">IF(B21=M21,TRUE(),FALSE())</f>
         <v>0</v>
       </c>
-      <c r="T21" s="0" t="s">
+      <c r="T21" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="U21" s="0" t="str">
+      <c r="U21" s="1" t="str">
         <f aca="false">IF(B21=M21,"All time high","")</f>
         <v/>
       </c>
@@ -2737,13 +2839,13 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W21" s="0" t="n">
+      <c r="W21" s="1" t="n">
         <v>2022</v>
       </c>
       <c r="X21" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="Y21" s="0" t="s">
+      <c r="Y21" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5774,6 +5876,14 @@
   <conditionalFormatting sqref="A1:AMJ1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>TRUE()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:AMJ21">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -5817,12 +5927,12 @@
   </sheetPr>
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J5" activeCellId="0" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5895,60 +6005,63 @@
       <c r="U1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>153</v>
       </c>
       <c r="K2" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>2011</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <f aca="false">2023-N2</f>
         <v>12</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="Q2" s="3" t="b">
         <f aca="false">IF(B2&lt;11,TRUE(),FALSE())</f>
@@ -5966,56 +6079,63 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U2" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V2" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="W2" s="0" t="s">
         <v>155</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" s="0" t="n">
+        <v>157</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="J3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="J3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="K3" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>2012</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <f aca="false">2023-N3</f>
         <v>11</v>
       </c>
-      <c r="P3" s="0" t="s">
-        <v>159</v>
+      <c r="P3" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="Q3" s="3" t="b">
         <f aca="false">IF(B3&lt;11,TRUE(),FALSE())</f>
@@ -6033,54 +6153,64 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U3" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V3" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="W3" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" s="0" t="n">
+        <v>162</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>182</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="J4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="J4" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K4" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <v>2013</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="O4" s="1" t="n">
         <f aca="false">2023-N4</f>
         <v>10</v>
       </c>
+      <c r="P4" s="0" t="s">
+        <v>165</v>
+      </c>
       <c r="Q4" s="3" t="b">
         <f aca="false">IF(B4&lt;11,TRUE(),FALSE())</f>
         <v>0</v>
@@ -6097,60 +6227,63 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U4" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V4" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="W4" s="0" t="s">
-        <v>155</v>
+        <v>166</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B5" s="0" t="n">
+        <v>167</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>183</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>167</v>
+      <c r="I5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="K5" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="M5" s="1" t="n">
         <v>2012</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5" s="1" t="n">
         <v>2003</v>
       </c>
-      <c r="O5" s="0" t="n">
+      <c r="O5" s="1" t="n">
         <f aca="false">2023-N5</f>
         <v>20</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="Q5" s="3" t="b">
         <f aca="false">IF(B5&lt;11,TRUE(),FALSE())</f>
@@ -6168,56 +6301,63 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U5" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V5" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="W5" s="0" t="s">
-        <v>155</v>
+        <v>171</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B6" s="0" t="n">
+        <v>172</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>178</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="H6" s="0" t="s">
+      <c r="F6" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="L6" s="0" t="n">
+      <c r="I6" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="K6" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M6" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="O6" s="0" t="n">
+      <c r="O6" s="8" t="n">
         <f aca="false">2023-N6</f>
         <v>5</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="Q6" s="3" t="b">
         <f aca="false">IF(B6&lt;11,TRUE(),FALSE())</f>
@@ -6235,60 +6375,63 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U6" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V6" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="W6" s="0" t="s">
-        <v>155</v>
+        <v>177</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B7" s="0" t="n">
+        <v>178</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>178</v>
+      <c r="I7" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="K7" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="1" t="n">
         <v>2011</v>
       </c>
-      <c r="O7" s="0" t="n">
+      <c r="O7" s="1" t="n">
         <f aca="false">2023-N7</f>
         <v>12</v>
       </c>
-      <c r="P7" s="0" t="s">
-        <v>179</v>
+      <c r="P7" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="Q7" s="3" t="b">
         <f aca="false">IF(B7&lt;11,TRUE(),FALSE())</f>
@@ -6306,62 +6449,66 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U7" s="0" t="n">
+      <c r="U7" s="1" t="n">
         <v>2022</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="W7" s="0" t="s">
-        <v>155</v>
+        <v>182</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>179</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="G8" s="0" t="s">
+      <c r="F8" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="L8" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="M8" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="N8" s="1" t="n">
         <v>2010</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="O8" s="1" t="n">
         <f aca="false">2023-N8</f>
         <v>13</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Q8" s="3" t="b">
         <f aca="false">IF(B8&lt;11,TRUE(),FALSE())</f>
@@ -6379,63 +6526,66 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U8" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V8" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="W8" s="0" t="s">
-        <v>155</v>
+        <v>188</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B9" s="0" t="n">
+        <v>189</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>181</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>189</v>
+      <c r="I9" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="K9" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M9" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N9" s="1" t="n">
         <v>2005</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="O9" s="1" t="n">
         <f aca="false">2023-N9</f>
         <v>18</v>
       </c>
-      <c r="P9" s="0" t="s">
-        <v>190</v>
+      <c r="P9" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="Q9" s="3" t="b">
         <f aca="false">IF(B9&lt;11,TRUE(),FALSE())</f>
@@ -6453,59 +6603,66 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U9" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V9" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="W9" s="0" t="s">
-        <v>155</v>
+        <v>193</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B10" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>170</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="L10" s="0" t="n">
+      <c r="I10" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K10" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="M10" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="N10" s="0" t="n">
+      <c r="N10" s="1" t="n">
         <v>2015</v>
       </c>
-      <c r="O10" s="0" t="n">
+      <c r="O10" s="1" t="n">
         <f aca="false">2023-N10</f>
         <v>8</v>
       </c>
-      <c r="P10" s="0" t="s">
-        <v>195</v>
+      <c r="P10" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="Q10" s="3" t="b">
         <f aca="false">IF(B10&lt;11,TRUE(),FALSE())</f>
@@ -6523,63 +6680,66 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U10" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V10" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="W10" s="0" t="s">
-        <v>155</v>
+        <v>198</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="B11" s="0" t="n">
+        <v>199</v>
+      </c>
+      <c r="B11" s="1" t="n">
         <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>199</v>
+      <c r="I11" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="K11" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="1" t="n">
         <v>2009</v>
       </c>
-      <c r="O11" s="0" t="n">
+      <c r="O11" s="1" t="n">
         <f aca="false">2023-N11</f>
         <v>14</v>
       </c>
-      <c r="P11" s="0" t="s">
-        <v>200</v>
+      <c r="P11" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="Q11" s="3" t="b">
         <f aca="false">IF(B11&lt;11,TRUE(),FALSE())</f>
@@ -6597,59 +6757,62 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U11" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V11" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="W11" s="0" t="s">
-        <v>155</v>
+        <v>203</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B12" s="0" t="n">
+        <v>204</v>
+      </c>
+      <c r="B12" s="1" t="n">
         <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="G12" s="0" t="s">
+      <c r="F12" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="L12" s="0" t="n">
+      <c r="I12" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="L12" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M12" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N12" s="1" t="n">
         <v>2013</v>
       </c>
-      <c r="O12" s="0" t="n">
+      <c r="O12" s="1" t="n">
         <f aca="false">2023-N12</f>
         <v>10</v>
       </c>
-      <c r="P12" s="0" t="s">
-        <v>206</v>
+      <c r="P12" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="Q12" s="3" t="b">
         <f aca="false">IF(B12&lt;11,TRUE(),FALSE())</f>
@@ -6667,60 +6830,63 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U12" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V12" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="W12" s="0" t="s">
-        <v>155</v>
+        <v>209</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="B13" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="B13" s="1" t="n">
         <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>174</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="H13" s="0" t="s">
+      <c r="G13" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>211</v>
+      <c r="I13" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="K13" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M13" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N13" s="1" t="n">
         <v>2009</v>
       </c>
-      <c r="O13" s="0" t="n">
+      <c r="O13" s="1" t="n">
         <f aca="false">2023-N13</f>
         <v>14</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="Q13" s="3" t="b">
         <f aca="false">IF(B13&lt;11,TRUE(),FALSE())</f>
@@ -6738,53 +6904,60 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U13" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V13" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="W13" s="0" t="s">
-        <v>155</v>
+        <v>215</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B14" s="0" t="n">
+        <v>216</v>
+      </c>
+      <c r="B14" s="1" t="n">
         <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>178</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="L14" s="0" t="n">
+      <c r="I14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K14" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="M14" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="N14" s="1" t="n">
         <v>2016</v>
       </c>
-      <c r="O14" s="0" t="n">
+      <c r="O14" s="1" t="n">
         <f aca="false">2023-N14</f>
         <v>7</v>
       </c>
-      <c r="P14" s="0" t="s">
-        <v>217</v>
+      <c r="P14" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="Q14" s="3" t="b">
         <f aca="false">IF(B14&lt;11,TRUE(),FALSE())</f>
@@ -6802,59 +6975,66 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U14" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V14" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="W14" s="0" t="s">
-        <v>155</v>
+        <v>220</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B15" s="0" t="n">
+        <v>221</v>
+      </c>
+      <c r="B15" s="1" t="n">
         <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="G15" s="0" t="s">
+      <c r="F15" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="L15" s="0" t="n">
+      <c r="I15" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="K15" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15" s="1" t="n">
         <v>2021</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="N15" s="1" t="n">
         <v>2013</v>
       </c>
-      <c r="O15" s="0" t="n">
+      <c r="O15" s="1" t="n">
         <f aca="false">2023-N15</f>
         <v>10</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="Q15" s="3" t="b">
         <f aca="false">IF(B15&lt;11,TRUE(),FALSE())</f>
@@ -6872,59 +7052,66 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U15" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V15" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="W15" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>225</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="B16" s="0" t="n">
+        <v>226</v>
+      </c>
+      <c r="B16" s="1" t="n">
         <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>181</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="L16" s="0" t="n">
+      <c r="I16" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="K16" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="M16" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="N16" s="1" t="n">
         <v>2016</v>
       </c>
-      <c r="O16" s="0" t="n">
+      <c r="O16" s="1" t="n">
         <f aca="false">2023-N16</f>
         <v>7</v>
       </c>
-      <c r="P16" s="0" t="s">
-        <v>227</v>
+      <c r="P16" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="Q16" s="3" t="b">
         <f aca="false">IF(B16&lt;11,TRUE(),FALSE())</f>
@@ -6942,57 +7129,60 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U16" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V16" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="W16" s="0" t="s">
-        <v>155</v>
+        <v>230</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="B17" s="0" t="n">
+        <v>231</v>
+      </c>
+      <c r="B17" s="1" t="n">
         <v>66</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>179</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="H17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="0" t="s">
-        <v>230</v>
+      <c r="I17" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="K17" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="L17" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="M17" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="N17" s="0" t="n">
+      <c r="N17" s="1" t="n">
         <v>2015</v>
       </c>
-      <c r="O17" s="0" t="n">
+      <c r="O17" s="1" t="n">
         <f aca="false">2023-N17</f>
         <v>8</v>
       </c>
-      <c r="P17" s="0" t="s">
-        <v>217</v>
+      <c r="P17" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="Q17" s="3" t="b">
         <f aca="false">IF(B17&lt;11,TRUE(),FALSE())</f>
@@ -7010,57 +7200,60 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U17" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V17" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="W17" s="0" t="s">
-        <v>155</v>
+        <v>234</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="B18" s="0" t="n">
+        <v>235</v>
+      </c>
+      <c r="B18" s="1" t="n">
         <v>319</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>170</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="H18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="0" t="s">
-        <v>234</v>
+      <c r="I18" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="K18" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L18" s="0" t="n">
+      <c r="L18" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="M18" s="0" t="n">
+      <c r="M18" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="N18" s="0" t="n">
+      <c r="N18" s="1" t="n">
         <v>2004</v>
       </c>
-      <c r="O18" s="0" t="n">
+      <c r="O18" s="1" t="n">
         <f aca="false">2023-N18</f>
         <v>19</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="Q18" s="3" t="b">
         <f aca="false">IF(B18&lt;11,TRUE(),FALSE())</f>
@@ -7078,63 +7271,66 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U18" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V18" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="W18" s="0" t="s">
-        <v>155</v>
+        <v>239</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="B19" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="B19" s="1" t="n">
         <v>83</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="H19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>240</v>
+      <c r="I19" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="K19" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L19" s="0" t="n">
+      <c r="L19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="M19" s="0" t="n">
+      <c r="M19" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="N19" s="0" t="n">
+      <c r="N19" s="1" t="n">
         <v>2004</v>
       </c>
-      <c r="O19" s="0" t="n">
+      <c r="O19" s="1" t="n">
         <f aca="false">2023-N19</f>
         <v>19</v>
       </c>
-      <c r="P19" s="0" t="s">
-        <v>241</v>
+      <c r="P19" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="Q19" s="3" t="b">
         <f aca="false">IF(B19&lt;11,TRUE(),FALSE())</f>
@@ -7152,63 +7348,63 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U19" s="0" t="n">
+      <c r="U19" s="1" t="n">
         <v>2019</v>
       </c>
       <c r="V19" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="W19" s="0" t="s">
-        <v>155</v>
+        <v>244</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B20" s="0" t="n">
+        <v>245</v>
+      </c>
+      <c r="B20" s="1" t="n">
         <v>81</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>178</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="H20" s="0" t="s">
+      <c r="F20" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>117</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="K20" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L20" s="0" t="n">
+      <c r="L20" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="M20" s="0" t="n">
+      <c r="M20" s="1" t="n">
         <v>2023</v>
       </c>
-      <c r="N20" s="0" t="n">
+      <c r="N20" s="1" t="n">
         <v>2009</v>
       </c>
-      <c r="O20" s="0" t="n">
+      <c r="O20" s="1" t="n">
         <f aca="false">2023-N20</f>
         <v>14</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="Q20" s="3" t="b">
         <f aca="false">IF(B20&lt;11,TRUE(),FALSE())</f>
@@ -7226,63 +7422,66 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U20" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V20" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="W20" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>249</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="B21" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="B21" s="1" t="n">
         <v>86</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>173</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="G21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="H21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>250</v>
+      <c r="I21" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="K21" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L21" s="0" t="n">
+      <c r="L21" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="M21" s="0" t="n">
+      <c r="M21" s="1" t="n">
         <v>2019</v>
       </c>
-      <c r="N21" s="0" t="n">
+      <c r="N21" s="1" t="n">
         <v>2009</v>
       </c>
-      <c r="O21" s="0" t="n">
+      <c r="O21" s="1" t="n">
         <f aca="false">2023-N21</f>
         <v>14</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="Q21" s="3" t="b">
         <f aca="false">IF(B21&lt;11,TRUE(),FALSE())</f>
@@ -7300,60 +7499,63 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U21" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V21" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="W21" s="0" t="s">
-        <v>155</v>
+        <v>254</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B22" s="0" t="n">
+        <v>255</v>
+      </c>
+      <c r="B22" s="1" t="n">
         <v>91</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>174</v>
       </c>
-      <c r="F22" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="H22" s="0" t="s">
+      <c r="F22" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>256</v>
+      <c r="I22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="K22" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L22" s="0" t="n">
+      <c r="L22" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="M22" s="0" t="n">
+      <c r="M22" s="1" t="n">
         <v>2016</v>
       </c>
-      <c r="N22" s="0" t="n">
+      <c r="N22" s="1" t="n">
         <v>2011</v>
       </c>
-      <c r="O22" s="0" t="n">
+      <c r="O22" s="1" t="n">
         <f aca="false">2023-N22</f>
         <v>12</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="Q22" s="3" t="b">
         <f aca="false">IF(B22&lt;11,TRUE(),FALSE())</f>
@@ -7371,59 +7573,66 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U22" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V22" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="W22" s="0" t="s">
-        <v>155</v>
+        <v>260</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="B23" s="0" t="n">
+        <v>261</v>
+      </c>
+      <c r="B23" s="1" t="n">
         <v>508</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>174</v>
       </c>
-      <c r="F23" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="G23" s="0" t="s">
+      <c r="F23" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="H23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="L23" s="0" t="n">
+      <c r="I23" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="K23" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="M23" s="0" t="n">
+      <c r="M23" s="1" t="n">
         <v>2017</v>
       </c>
-      <c r="N23" s="0" t="n">
+      <c r="N23" s="1" t="n">
         <v>2008</v>
       </c>
-      <c r="O23" s="0" t="n">
+      <c r="O23" s="1" t="n">
         <f aca="false">2023-N23</f>
         <v>15</v>
       </c>
-      <c r="P23" s="0" t="s">
-        <v>263</v>
+      <c r="P23" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="Q23" s="3" t="b">
         <f aca="false">IF(B23&lt;11,TRUE(),FALSE())</f>
@@ -7441,11 +7650,14 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="U23" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V23" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="W23" s="0" t="s">
-        <v>155</v>
+        <v>266</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -7454,9 +7666,17 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:AMJ1048576">
+  <conditionalFormatting sqref="A1:AMJ1 A2:O2 V2:AMJ6 A3:U6 Q2:U2 A7:AMJ1048576">
     <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>TRUE()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:W1 A2:O2 V2:W6 A3:U6 Q2:U2 A7:W23">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -7491,7 +7711,7 @@
     <hyperlink ref="V20" r:id="rId19" display="https://libema-open.nl/wp-content/uploads/2023/05/fNpQoEOl.webp"/>
     <hyperlink ref="V21" r:id="rId20" display="https://libema-open.nl/wp-content/uploads/2023/05/ODTCCbpp.webp"/>
     <hyperlink ref="V22" r:id="rId21" display="https://libema-open.nl/wp-content/uploads/2023/05/Friedsam_Crop.webp"/>
-    <hyperlink ref="V23" r:id="rId22" display="https://libema-open.nl/wp-content/uploads/2023/05/ODTCCbpp.webp"/>
+    <hyperlink ref="V23" r:id="rId22" display="https://libema-open.nl/wp-content/uploads/2023/05/Svitolina_Hero-Smile.webp"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -7521,7 +7741,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Init discrete slider for preference strength selection
</commit_message>
<xml_diff>
--- a/backend/data/Competitors.xlsx
+++ b/backend/data/Competitors.xlsx
@@ -156,7 +156,7 @@
     <t xml:space="preserve">Forehand</t>
   </si>
   <si>
-    <t xml:space="preserve">mr. nice guy, powerful serve, powerful forehand, athletic, powerful, emotiona</t>
+    <t xml:space="preserve">mr. nice guy, powerful serve, powerful forehand, athletic, powerful, emotional</t>
   </si>
   <si>
     <t xml:space="preserve">Auger-Aliassime is an athletic player with a complete game. His serve and forehand are his biggest weapons, but he's also known for his speed and agility, allowing him to defend well. He's still maturing in terms of strategy, but his raw talent and physical attributes make him a serious threat.</t>
@@ -546,7 +546,7 @@
     <t xml:space="preserve">CH</t>
   </si>
   <si>
-    <t xml:space="preserve">olympian, groundstroke, tactical, defensive, serve, footwork</t>
+    <t xml:space="preserve">olympian, groundstrokes, tactical, defensive, serve, footwork</t>
   </si>
   <si>
     <t xml:space="preserve">Bencic possesses a versatile game marked by excellent court coverage and an ability to change direction of the ball with ease. Her smart tactical sense allows her to construct points effectively, often outmaneuvering her opponents with precise shot placement.</t>
@@ -618,7 +618,7 @@
     <t xml:space="preserve">Asia</t>
   </si>
   <si>
-    <t xml:space="preserve">talented, versatile, strong groundstrokes, powerful serve, aggressive, net play</t>
+    <t xml:space="preserve">talented, versatile, groundstrokes, serve, aggressive, net play</t>
   </si>
   <si>
     <t xml:space="preserve">Zheng is a young player known for her aggressive game style, with a powerful serve and strong groundstrokes. She often looks to dictate the play and isn't afraid to go for winners.</t>
@@ -654,7 +654,7 @@
     <t xml:space="preserve">BE</t>
   </si>
   <si>
-    <t xml:space="preserve">lovely, respectful, interactive, consistent, footwork, groundstrokes, serve, defensive</t>
+    <t xml:space="preserve"> respectful, interactive, consistent, footwork, groundstrokes, serve, defensive</t>
   </si>
   <si>
     <t xml:space="preserve">Mertens has a well-rounded game, marked by solid groundstrokes, good court coverage and tactical intelligence. Her versatile game allows her to adapt to different playing styles and court surfaces.</t>
@@ -783,7 +783,7 @@
     <t xml:space="preserve">Caty Mcnally</t>
   </si>
   <si>
-    <t xml:space="preserve">aggressive, strong serve, versatile, doubles strength, net game</t>
+    <t xml:space="preserve">aggressive, powerful serve, versatile, doubles strength, net game</t>
   </si>
   <si>
     <t xml:space="preserve">Known for her aggressive style and strong serve, Caty McNally is a versatile player who can excel on various surfaces. She's made a name for herself in doubles, often partnering with fellow American Coco Gauff, and has started to break through in singles as well. With a potent one-two punch of a big serve followed by a heavy groundstroke, McNally can quickly take control of points. She also possesses a rare weapon in the women's game: a strong net game, thanks to her doubles expertise.”</t>
@@ -798,7 +798,7 @@
     <t xml:space="preserve">Anna Blinkova</t>
   </si>
   <si>
-    <t xml:space="preserve">aggressive, all-court player, powerful groundstrokes</t>
+    <t xml:space="preserve">aggressive, all-court player, groundstrokes</t>
   </si>
   <si>
     <t xml:space="preserve">Anna Blinkova is a solid all-court player known for her powerful groundstrokes. Her aggressive style of play often sees her taking the ball on the rise and aiming for the lines. Blinkova has shown that she can compete at the top level and has recorded victories against higher-ranked opponents. Her ability to generate power from both wings and her willingness to attack and dictate play are key elements of her game.”</t>
@@ -825,7 +825,7 @@
     <t xml:space="preserve">Alison Riske-Amritraj</t>
   </si>
   <si>
-    <t xml:space="preserve">aggressive, positive, powerful groundstrokes, strong serve, net play, tough competitor</t>
+    <t xml:space="preserve">aggressive, positive, groundstrokes, strong serve, net play, tough competitor</t>
   </si>
   <si>
     <t xml:space="preserve">Alison Riske-Amritraj is known for her aggressive baseline play and powerful groundstrokes. Her strengths include a strong serve and a particularly effective backhand. She also has a knack for coming to the net, showcasing her versatile skill set. Over the years, Riske-Amritraj has developed a reputation for being a tough competitor, often playing her best tennis in tight situations.</t>
@@ -855,7 +855,7 @@
     <t xml:space="preserve">Rebecca Peterson</t>
   </si>
   <si>
-    <t xml:space="preserve">baseline player, consistent, strong groundstrokes, defensive, counterpunching, fighting spirit</t>
+    <t xml:space="preserve">baseline player, consistent, groundstrokes, defensive, counterpunching, fighting spirit</t>
   </si>
   <si>
     <t xml:space="preserve">Rebecca Peterson is a solid baseline player with a consistent game. She uses her strong groundstrokes to construct points and can change direction of the ball effectively. Peterson also has a good defensive game, often turning defense into offense with her counterpunching ability. She's known for her fighting spirit on the court, often grinding out tough matches.</t>
@@ -897,7 +897,7 @@
     <t xml:space="preserve">UA</t>
   </si>
   <si>
-    <t xml:space="preserve">consistent, excellent movement, defensive skills, solid groundstrokes, mental toughness, competitive spirit</t>
+    <t xml:space="preserve">consistent, excellent movement, defensive skills, groundstrokes, mental toughness, competitive spirit</t>
   </si>
   <si>
     <t xml:space="preserve">Elina Svitolina is one of the most consistent players on the WTA Tour, known for her excellent movement, strong defensive skills, and the ability to turn defense into offense. Her game is based around her solid groundstrokes and her ability to move her opponents around the court. Svitolina is also known for her mental toughness and strong competitive spirit, often elevating her game in important moments.</t>
@@ -1157,14 +1157,14 @@
   <dimension ref="A1:AA1021"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L5" activeCellId="0" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.45"/>
@@ -6131,14 +6131,14 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="18.34"/>
@@ -7707,7 +7707,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>275</v>
       </c>
@@ -8027,7 +8027,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.45"/>
   </cols>

</xml_diff>

<commit_message>
Get filtered parameter players from BE
</commit_message>
<xml_diff>
--- a/backend/data/Competitors.xlsx
+++ b/backend/data/Competitors.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="395">
   <si>
     <t xml:space="preserve">Player</t>
   </si>
@@ -917,9 +917,6 @@
   </si>
   <si>
     <t xml:space="preserve">Aliaksandra Sasnovich</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Backhand down the line</t>
   </si>
   <si>
     <t xml:space="preserve">versatile, groundstrokes, serve, consistency, tactical</t>
@@ -1552,7 +1549,7 @@
       <selection pane="bottomRight" activeCell="Z25" activeCellId="0" sqref="Z25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.45"/>
@@ -7569,14 +7566,14 @@
   <dimension ref="A1:Z44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W7" activeCellId="0" sqref="W7"/>
+      <selection pane="bottomRight" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="18.34"/>
@@ -8560,16 +8557,16 @@
         <v>174</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>283</v>
+        <v>10</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K13" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="M13" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -8589,7 +8586,7 @@
         <v>14</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="S13" s="2" t="n">
         <f aca="false">IF(B13&lt;11,TRUE(),FALSE())</f>
@@ -8612,7 +8609,7 @@
       </c>
       <c r="X13" s="1"/>
       <c r="Y13" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Z13" s="1" t="s">
         <v>226</v>
@@ -8620,7 +8617,7 @@
     </row>
     <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>44</v>
@@ -8638,10 +8635,10 @@
         <v>30</v>
       </c>
       <c r="K14" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="M14" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -8661,7 +8658,7 @@
         <v>7</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="S14" s="2" t="n">
         <f aca="false">IF(B14&lt;11,TRUE(),FALSE())</f>
@@ -8684,7 +8681,7 @@
       </c>
       <c r="X14" s="1"/>
       <c r="Y14" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Z14" s="1" t="s">
         <v>226</v>
@@ -8692,7 +8689,7 @@
     </row>
     <row r="15" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>42</v>
@@ -8722,10 +8719,10 @@
         <v>30</v>
       </c>
       <c r="K15" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="M15" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -8745,7 +8742,7 @@
         <v>10</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="S15" s="2" t="n">
         <f aca="false">IF(B15&lt;11,TRUE(),FALSE())</f>
@@ -8768,7 +8765,7 @@
       </c>
       <c r="X15" s="1"/>
       <c r="Y15" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="Z15" s="1" t="s">
         <v>226</v>
@@ -8776,7 +8773,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>22</v>
@@ -8806,10 +8803,10 @@
         <v>30</v>
       </c>
       <c r="K16" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="M16" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -8829,7 +8826,7 @@
         <v>7</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="S16" s="2" t="n">
         <f aca="false">IF(B16&lt;11,TRUE(),FALSE())</f>
@@ -8852,7 +8849,7 @@
       </c>
       <c r="X16" s="1"/>
       <c r="Y16" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Z16" s="1" t="s">
         <v>226</v>
@@ -8860,7 +8857,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>66</v>
@@ -8878,10 +8875,10 @@
         <v>30</v>
       </c>
       <c r="K17" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="L17" s="7" t="s">
         <v>304</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>305</v>
       </c>
       <c r="M17" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -8901,7 +8898,7 @@
         <v>8</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="S17" s="2" t="n">
         <f aca="false">IF(B17&lt;11,TRUE(),FALSE())</f>
@@ -8924,7 +8921,7 @@
       </c>
       <c r="X17" s="1"/>
       <c r="Y17" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Z17" s="1" t="s">
         <v>226</v>
@@ -8932,7 +8929,7 @@
     </row>
     <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>319</v>
@@ -8950,10 +8947,10 @@
         <v>30</v>
       </c>
       <c r="K18" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="L18" s="7" t="s">
         <v>308</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>309</v>
       </c>
       <c r="M18" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -8973,7 +8970,7 @@
         <v>19</v>
       </c>
       <c r="R18" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S18" s="2" t="n">
         <f aca="false">IF(B18&lt;11,TRUE(),FALSE())</f>
@@ -8996,7 +8993,7 @@
       </c>
       <c r="X18" s="1"/>
       <c r="Y18" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Z18" s="1" t="s">
         <v>226</v>
@@ -9004,7 +9001,7 @@
     </row>
     <row r="19" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>83</v>
@@ -9034,10 +9031,10 @@
         <v>30</v>
       </c>
       <c r="K19" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>314</v>
       </c>
       <c r="M19" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -9057,7 +9054,7 @@
         <v>19</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S19" s="2" t="n">
         <f aca="false">IF(B19&lt;11,TRUE(),FALSE())</f>
@@ -9080,7 +9077,7 @@
       </c>
       <c r="X19" s="1"/>
       <c r="Y19" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Z19" s="1" t="s">
         <v>226</v>
@@ -9088,7 +9085,7 @@
     </row>
     <row r="20" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>81</v>
@@ -9115,10 +9112,10 @@
         <v>134</v>
       </c>
       <c r="K20" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>319</v>
       </c>
       <c r="M20" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -9138,7 +9135,7 @@
         <v>14</v>
       </c>
       <c r="R20" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="S20" s="2" t="n">
         <f aca="false">IF(B20&lt;11,TRUE(),FALSE())</f>
@@ -9161,7 +9158,7 @@
       </c>
       <c r="X20" s="1"/>
       <c r="Y20" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Z20" s="1" t="s">
         <v>226</v>
@@ -9169,7 +9166,7 @@
     </row>
     <row r="21" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>86</v>
@@ -9199,10 +9196,10 @@
         <v>30</v>
       </c>
       <c r="K21" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="M21" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -9222,7 +9219,7 @@
         <v>14</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="S21" s="2" t="n">
         <f aca="false">IF(B21&lt;11,TRUE(),FALSE())</f>
@@ -9245,7 +9242,7 @@
       </c>
       <c r="X21" s="1"/>
       <c r="Y21" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="Z21" s="1" t="s">
         <v>226</v>
@@ -9253,7 +9250,7 @@
     </row>
     <row r="22" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>91</v>
@@ -9268,10 +9265,10 @@
         <v>174</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>329</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>132</v>
@@ -9280,10 +9277,10 @@
         <v>30</v>
       </c>
       <c r="K22" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>331</v>
       </c>
       <c r="M22" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -9303,7 +9300,7 @@
         <v>12</v>
       </c>
       <c r="R22" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="S22" s="2" t="n">
         <f aca="false">IF(B22&lt;11,TRUE(),FALSE())</f>
@@ -9326,7 +9323,7 @@
       </c>
       <c r="X22" s="1"/>
       <c r="Y22" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Z22" s="1" t="s">
         <v>226</v>
@@ -9334,7 +9331,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>508</v>
@@ -9349,10 +9346,10 @@
         <v>174</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>336</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>147</v>
@@ -9364,10 +9361,10 @@
         <v>30</v>
       </c>
       <c r="K23" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="M23" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -9387,7 +9384,7 @@
         <v>15</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="S23" s="2" t="n">
         <f aca="false">IF(B23&lt;11,TRUE(),FALSE())</f>
@@ -9410,7 +9407,7 @@
       </c>
       <c r="X23" s="1"/>
       <c r="Y23" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Z23" s="1" t="s">
         <v>226</v>
@@ -9418,7 +9415,7 @@
     </row>
     <row r="24" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B24" s="9" t="n">
         <v>92</v>
@@ -9459,7 +9456,7 @@
         <v>5</v>
       </c>
       <c r="R24" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="S24" s="10" t="n">
         <f aca="false">IF(B24&lt;11,TRUE(),FALSE())</f>
@@ -9482,7 +9479,7 @@
         <v>172</v>
       </c>
       <c r="Y24" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Z24" s="15" t="s">
         <v>226</v>
@@ -9490,7 +9487,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>98</v>
@@ -9502,10 +9499,10 @@
         <v>178</v>
       </c>
       <c r="F25" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="G25" s="0" t="s">
         <v>345</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>346</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>50</v>
@@ -9550,7 +9547,7 @@
         <v>172</v>
       </c>
       <c r="Y25" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="Z25" s="1" t="s">
         <v>226</v>
@@ -9558,7 +9555,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>110</v>
@@ -9602,7 +9599,7 @@
         <v>10</v>
       </c>
       <c r="R26" s="0" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="S26" s="2" t="n">
         <f aca="false">IF(B26&lt;11,TRUE(),FALSE())</f>
@@ -9624,7 +9621,7 @@
         <v>172</v>
       </c>
       <c r="Y26" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Z26" s="1" t="s">
         <v>226</v>
@@ -9632,7 +9629,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>116</v>
@@ -9692,7 +9689,7 @@
         <v>172</v>
       </c>
       <c r="Y27" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Z27" s="1" t="s">
         <v>226</v>
@@ -9700,7 +9697,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>56</v>
@@ -9744,7 +9741,7 @@
         <v>10</v>
       </c>
       <c r="R28" s="0" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="S28" s="2" t="n">
         <f aca="false">IF(B28&lt;11,TRUE(),FALSE())</f>
@@ -9766,7 +9763,7 @@
         <v>172</v>
       </c>
       <c r="Y28" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Z28" s="1" t="s">
         <v>226</v>
@@ -9774,7 +9771,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>123</v>
@@ -9834,7 +9831,7 @@
         <v>172</v>
       </c>
       <c r="Y29" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Z29" s="1" t="s">
         <v>226</v>
@@ -9842,7 +9839,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>106</v>
@@ -9854,10 +9851,10 @@
         <v>180</v>
       </c>
       <c r="F30" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>358</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>359</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>50</v>
@@ -9883,7 +9880,7 @@
         <v>10</v>
       </c>
       <c r="R30" s="0" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="S30" s="2" t="n">
         <f aca="false">IF(B30&lt;11,TRUE(),FALSE())</f>
@@ -9905,7 +9902,7 @@
         <v>172</v>
       </c>
       <c r="Y30" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Z30" s="1" t="s">
         <v>226</v>
@@ -9913,7 +9910,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>89</v>
@@ -9954,7 +9951,7 @@
         <v>18</v>
       </c>
       <c r="R31" s="0" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="S31" s="2" t="n">
         <f aca="false">IF(B31&lt;11,TRUE(),FALSE())</f>
@@ -9976,7 +9973,7 @@
         <v>172</v>
       </c>
       <c r="Y31" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="Z31" s="1" t="s">
         <v>226</v>
@@ -9984,7 +9981,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>142</v>
@@ -10035,7 +10032,7 @@
         <v>172</v>
       </c>
       <c r="Y32" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Z32" s="1" t="s">
         <v>226</v>
@@ -10043,7 +10040,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>154</v>
@@ -10087,7 +10084,7 @@
         <v>10</v>
       </c>
       <c r="R33" s="0" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S33" s="2" t="n">
         <f aca="false">IF(B33&lt;11,TRUE(),FALSE())</f>
@@ -10109,7 +10106,7 @@
         <v>172</v>
       </c>
       <c r="Y33" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Z33" s="1" t="s">
         <v>226</v>
@@ -10117,7 +10114,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>156</v>
@@ -10129,10 +10126,10 @@
         <v>165</v>
       </c>
       <c r="F34" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G34" s="0" t="s">
         <v>328</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>329</v>
       </c>
       <c r="H34" s="0" t="s">
         <v>132</v>
@@ -10158,7 +10155,7 @@
         <v>5</v>
       </c>
       <c r="R34" s="0" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="S34" s="2" t="n">
         <f aca="false">IF(B34&lt;11,TRUE(),FALSE())</f>
@@ -10180,7 +10177,7 @@
         <v>172</v>
       </c>
       <c r="Y34" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="Z34" s="1" t="s">
         <v>226</v>
@@ -10188,7 +10185,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>114</v>
@@ -10248,7 +10245,7 @@
         <v>172</v>
       </c>
       <c r="Y35" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="Z35" s="1" t="s">
         <v>226</v>
@@ -10256,7 +10253,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>165</v>
@@ -10297,7 +10294,7 @@
         <v>16</v>
       </c>
       <c r="R36" s="0" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S36" s="2" t="n">
         <f aca="false">IF(B36&lt;11,TRUE(),FALSE())</f>
@@ -10319,7 +10316,7 @@
         <v>172</v>
       </c>
       <c r="Y36" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="Z36" s="1" t="s">
         <v>226</v>
@@ -10327,7 +10324,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>170</v>
@@ -10374,7 +10371,7 @@
         <v>13</v>
       </c>
       <c r="R37" s="0" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="S37" s="2" t="n">
         <f aca="false">IF(B37&lt;11,TRUE(),FALSE())</f>
@@ -10396,7 +10393,7 @@
         <v>172</v>
       </c>
       <c r="Y37" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="Z37" s="1" t="s">
         <v>226</v>
@@ -10404,7 +10401,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>173</v>
@@ -10445,7 +10442,7 @@
         <v>11</v>
       </c>
       <c r="R38" s="0" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="S38" s="2" t="n">
         <f aca="false">IF(B38&lt;11,TRUE(),FALSE())</f>
@@ -10467,7 +10464,7 @@
         <v>172</v>
       </c>
       <c r="Y38" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="Z38" s="1" t="s">
         <v>226</v>
@@ -10475,7 +10472,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>178</v>
@@ -10535,7 +10532,7 @@
         <v>172</v>
       </c>
       <c r="Y39" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Z39" s="1" t="s">
         <v>226</v>
@@ -10543,7 +10540,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>148</v>
@@ -10603,7 +10600,7 @@
         <v>172</v>
       </c>
       <c r="Y40" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Z40" s="1" t="s">
         <v>226</v>
@@ -10611,7 +10608,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>159</v>
@@ -10623,10 +10620,10 @@
         <v>164</v>
       </c>
       <c r="F41" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="G41" s="0" t="s">
         <v>386</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>387</v>
       </c>
       <c r="H41" s="0" t="s">
         <v>245</v>
@@ -10652,7 +10649,7 @@
         <v>7</v>
       </c>
       <c r="R41" s="0" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S41" s="2" t="n">
         <f aca="false">IF(B41&lt;11,TRUE(),FALSE())</f>
@@ -10674,7 +10671,7 @@
         <v>172</v>
       </c>
       <c r="Y41" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Z41" s="1" t="s">
         <v>226</v>
@@ -10682,7 +10679,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>194</v>
@@ -10694,10 +10691,10 @@
         <v>188</v>
       </c>
       <c r="F42" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="G42" s="0" t="s">
         <v>390</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>391</v>
       </c>
       <c r="H42" s="0" t="s">
         <v>65</v>
@@ -10742,7 +10739,7 @@
         <v>172</v>
       </c>
       <c r="Y42" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Z42" s="1" t="s">
         <v>226</v>
@@ -10750,7 +10747,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>197</v>
@@ -10810,7 +10807,7 @@
         <v>172</v>
       </c>
       <c r="Y43" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Z43" s="1" t="s">
         <v>226</v>
@@ -10818,7 +10815,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>210</v>
@@ -10859,7 +10856,7 @@
         <v>15</v>
       </c>
       <c r="R44" s="0" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="S44" s="2" t="n">
         <f aca="false">IF(B44&lt;11,TRUE(),FALSE())</f>
@@ -10881,7 +10878,7 @@
         <v>217</v>
       </c>
       <c r="Y44" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Z44" s="1" t="s">
         <v>226</v>
@@ -10939,27 +10936,27 @@
     <hyperlink ref="Y21" r:id="rId20" display="https://libema-open.nl/wp-content/uploads/2023/05/ODTCCbpp.webp"/>
     <hyperlink ref="Y22" r:id="rId21" display="https://libema-open.nl/wp-content/uploads/2023/05/Friedsam_Crop.webp"/>
     <hyperlink ref="Y23" r:id="rId22" display="https://libema-open.nl/wp-content/uploads/2023/05/Svitolina_Hero-Smile.webp"/>
-    <hyperlink ref="Y24" r:id="rId23" display="https://libema-open.nl"/>
-    <hyperlink ref="Y25" r:id="rId24" display="https://libema-open.nl"/>
-    <hyperlink ref="Y26" r:id="rId25" display="https://libema-open.nl"/>
-    <hyperlink ref="Y27" r:id="rId26" display="https://libema-open.nl"/>
-    <hyperlink ref="Y28" r:id="rId27" display="https://libema-open.nl"/>
-    <hyperlink ref="Y29" r:id="rId28" display="https://libema-open.nl"/>
-    <hyperlink ref="Y30" r:id="rId29" display="https://libema-open.nl"/>
-    <hyperlink ref="Y31" r:id="rId30" display="https://libema-open.nl"/>
-    <hyperlink ref="Y32" r:id="rId31" display="https://libema-open.nl"/>
-    <hyperlink ref="Y33" r:id="rId32" display="https://libema-open.nl"/>
-    <hyperlink ref="Y34" r:id="rId33" display="https://libema-open.nl"/>
-    <hyperlink ref="Y35" r:id="rId34" display="https://libema-open.nl"/>
-    <hyperlink ref="Y36" r:id="rId35" display="https://libema-open.nl"/>
-    <hyperlink ref="Y37" r:id="rId36" display="https://libema-open.nl"/>
-    <hyperlink ref="Y38" r:id="rId37" display="https://libema-open.nl"/>
-    <hyperlink ref="Y39" r:id="rId38" display="https://libema-open.nl"/>
-    <hyperlink ref="Y40" r:id="rId39" display="https://libema-open.nl"/>
-    <hyperlink ref="Y41" r:id="rId40" display="https://libema-open.nl"/>
-    <hyperlink ref="Y42" r:id="rId41" display="https://libema-open.nl"/>
-    <hyperlink ref="Y43" r:id="rId42" display="https://libema-open.nl"/>
-    <hyperlink ref="Y44" r:id="rId43" display="https://libema-open.nl"/>
+    <hyperlink ref="Y24" r:id="rId23" display="https://libema-open.nl/wp-content/uploads/2023/05/Volynets_crop.webp"/>
+    <hyperlink ref="Y25" r:id="rId24" display="https://libema-open.nl/wp-content/uploads/2023/05/Galfi_crop.webp"/>
+    <hyperlink ref="Y26" r:id="rId25" display="https://libema-open.nl/wp-content/uploads/2023/05/player-placeholder.png"/>
+    <hyperlink ref="Y27" r:id="rId26" display="https://libema-open.nl/wp-content/uploads/2023/05/Yuan_crop.webp"/>
+    <hyperlink ref="Y28" r:id="rId27" display="https://libema-open.nl/wp-content/uploads/2023/05/Minnen_crop.webp"/>
+    <hyperlink ref="Y29" r:id="rId28" display="https://libema-open.nl/wp-content/uploads/2023/05/player-placeholder.png"/>
+    <hyperlink ref="Y30" r:id="rId29" display="https://libema-open.nl/wp-content/uploads/2023/05/Hruncakova_crop.webp"/>
+    <hyperlink ref="Y31" r:id="rId30" display="https://libema-open.nl/wp-content/uploads/2023/05/Wickmayer_crop.webp"/>
+    <hyperlink ref="Y32" r:id="rId31" display="https://libema-open.nl/wp-content/uploads/2023/05/player-placeholder.png"/>
+    <hyperlink ref="Y33" r:id="rId32" display="https://libema-open.nl/wp-content/uploads/2023/05/Hon_crop.webp"/>
+    <hyperlink ref="Y34" r:id="rId33" display="https://libema-open.nl/wp-content/uploads/2023/05/Lys_crop.webp"/>
+    <hyperlink ref="Y35" r:id="rId34" display="https://libema-open.nl/wp-content/uploads/2023/05/Krueger_crop.webp"/>
+    <hyperlink ref="Y36" r:id="rId35" display="https://libema-open.nl/wp-content/uploads/2023/05/Vandeweghe_crop.webp"/>
+    <hyperlink ref="Y37" r:id="rId36" display="https://libema-open.nl/wp-content/uploads/2023/05/Vickery_crop.webp"/>
+    <hyperlink ref="Y38" r:id="rId37" display="https://libema-open.nl/wp-content/uploads/2023/05/Konjuh_crop.webp"/>
+    <hyperlink ref="Y39" r:id="rId38" display="https://libema-open.nl/wp-content/uploads/2023/05/Zhao_crop.webp"/>
+    <hyperlink ref="Y40" r:id="rId39" display="https://libema-open.nl/wp-content/uploads/2023/05/player-placeholder.png"/>
+    <hyperlink ref="Y41" r:id="rId40" display="https://libema-open.nl/wp-content/uploads/2023/05/player-placeholder.png"/>
+    <hyperlink ref="Y42" r:id="rId41" display="https://libema-open.nl/wp-content/uploads/2023/05/player-placeholder.png"/>
+    <hyperlink ref="Y43" r:id="rId42" display="https://libema-open.nl/wp-content/uploads/2023/05/player-placeholder.png"/>
+    <hyperlink ref="Y44" r:id="rId43" display="https://libema-open.nl/wp-content/uploads/2023/05/player-placeholder.png"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -10982,14 +10979,14 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>